<commit_message>
FInishing for first demo
</commit_message>
<xml_diff>
--- a/Werkwoorden_Lijst.xlsx
+++ b/Werkwoorden_Lijst.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -43,6 +43,11 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -73,17 +78,20 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -387,13 +395,13 @@
   </sheetPr>
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A118" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="B123" activeCellId="0" pane="topLeft" sqref="B123:C123"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
+      <selection activeCell="B139" activeCellId="0" pane="topLeft" sqref="B139:F166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="3" min="3" style="2" width="24.68"/>
+    <col customWidth="1" max="3" min="3" style="2" width="15.91"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="3">
@@ -585,7 +593,11 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="8" s="3">
-      <c r="A8" s="2" t="inlineStr"/>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>doe</t>
+        </is>
+      </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
           <t>doen</t>
@@ -3445,239 +3457,1028 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="123" s="3">
-      <c r="A123" s="2" t="inlineStr"/>
-      <c r="B123" s="2" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" s="2" t="inlineStr"/>
-      <c r="E123" s="2" t="inlineStr"/>
-      <c r="F123" s="2" t="inlineStr"/>
+      <c r="B123" s="2" t="inlineStr">
+        <is>
+          <t>staan</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="inlineStr">
+        <is>
+          <t>stond, stonden</t>
+        </is>
+      </c>
+      <c r="E123" s="2" t="inlineStr">
+        <is>
+          <t>gestaan</t>
+        </is>
+      </c>
+      <c r="F123" s="2" t="inlineStr">
+        <is>
+          <t>stand</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="124" s="3">
-      <c r="B124" s="2" t="n"/>
-      <c r="E124" s="2" t="n"/>
-      <c r="F124" s="2" t="n"/>
+      <c r="B124" s="2" t="inlineStr">
+        <is>
+          <t>steken</t>
+        </is>
+      </c>
+      <c r="C124" s="2" t="inlineStr">
+        <is>
+          <t>stak, staken</t>
+        </is>
+      </c>
+      <c r="E124" s="2" t="inlineStr">
+        <is>
+          <t>gestoken</t>
+        </is>
+      </c>
+      <c r="F124" s="2" t="inlineStr">
+        <is>
+          <t>stab, sting</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="125" s="3">
-      <c r="B125" s="2" t="n"/>
-      <c r="E125" s="2" t="n"/>
-      <c r="F125" s="2" t="n"/>
+      <c r="B125" s="2" t="inlineStr">
+        <is>
+          <t>stelen</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="inlineStr">
+        <is>
+          <t>stal, stalen</t>
+        </is>
+      </c>
+      <c r="E125" s="2" t="inlineStr">
+        <is>
+          <t>gestolen</t>
+        </is>
+      </c>
+      <c r="F125" s="2" t="inlineStr">
+        <is>
+          <t>steal</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="126" s="3">
-      <c r="B126" s="2" t="n"/>
-      <c r="D126" s="2" t="n"/>
-      <c r="E126" s="2" t="n"/>
-      <c r="F126" s="2" t="n"/>
+      <c r="B126" s="2" t="inlineStr">
+        <is>
+          <t>sterven</t>
+        </is>
+      </c>
+      <c r="C126" s="2" t="inlineStr">
+        <is>
+          <t>stierf, stierven</t>
+        </is>
+      </c>
+      <c r="D126" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E126" s="2" t="inlineStr">
+        <is>
+          <t>gestorven</t>
+        </is>
+      </c>
+      <c r="F126" s="2" t="inlineStr">
+        <is>
+          <t>die</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="127" s="3">
-      <c r="B127" s="2" t="n"/>
-      <c r="D127" s="2" t="n"/>
-      <c r="E127" s="2" t="n"/>
-      <c r="F127" s="2" t="n"/>
+      <c r="B127" s="2" t="inlineStr">
+        <is>
+          <t>stijgen</t>
+        </is>
+      </c>
+      <c r="C127" s="2" t="inlineStr">
+        <is>
+          <t>steeg, stegen</t>
+        </is>
+      </c>
+      <c r="D127" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E127" s="2" t="inlineStr">
+        <is>
+          <t>isgestegen</t>
+        </is>
+      </c>
+      <c r="F127" s="2" t="inlineStr">
+        <is>
+          <t>climb</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="128" s="3">
-      <c r="B128" s="2" t="n"/>
-      <c r="D128" s="2" t="n"/>
-      <c r="E128" s="2" t="n"/>
-      <c r="F128" s="2" t="n"/>
+      <c r="B128" s="2" t="inlineStr">
+        <is>
+          <t>treden</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="inlineStr">
+        <is>
+          <t>trad, traden</t>
+        </is>
+      </c>
+      <c r="D128" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E128" s="2" t="inlineStr">
+        <is>
+          <t>getreden</t>
+        </is>
+      </c>
+      <c r="F128" s="2" t="inlineStr">
+        <is>
+          <t>step</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="129" s="3">
-      <c r="B129" s="2" t="n"/>
-      <c r="E129" s="2" t="n"/>
-      <c r="F129" s="2" t="n"/>
+      <c r="B129" s="2" t="inlineStr">
+        <is>
+          <t>treffen</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="inlineStr">
+        <is>
+          <t>trof, troffen</t>
+        </is>
+      </c>
+      <c r="E129" s="2" t="inlineStr">
+        <is>
+          <t>getroffen</t>
+        </is>
+      </c>
+      <c r="F129" s="2" t="inlineStr">
+        <is>
+          <t>hit</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="130" s="3">
-      <c r="B130" s="2" t="n"/>
-      <c r="E130" s="2" t="n"/>
-      <c r="F130" s="2" t="n"/>
+      <c r="B130" s="2" t="inlineStr">
+        <is>
+          <t>trekken</t>
+        </is>
+      </c>
+      <c r="C130" s="2" t="inlineStr">
+        <is>
+          <t>trok, trokken</t>
+        </is>
+      </c>
+      <c r="E130" s="2" t="inlineStr">
+        <is>
+          <t>getrokken</t>
+        </is>
+      </c>
+      <c r="F130" s="2" t="inlineStr">
+        <is>
+          <t>pull</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="131" s="3">
-      <c r="B131" s="2" t="n"/>
-      <c r="D131" s="2" t="n"/>
-      <c r="E131" s="2" t="n"/>
-      <c r="F131" s="2" t="n"/>
+      <c r="B131" s="2" t="inlineStr">
+        <is>
+          <t>vallen</t>
+        </is>
+      </c>
+      <c r="C131" s="2" t="inlineStr">
+        <is>
+          <t>viel, vielen</t>
+        </is>
+      </c>
+      <c r="D131" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E131" s="2" t="inlineStr">
+        <is>
+          <t>gevallen</t>
+        </is>
+      </c>
+      <c r="F131" s="2" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="132" s="3">
-      <c r="B132" s="2" t="n"/>
-      <c r="E132" s="2" t="n"/>
-      <c r="F132" s="2" t="n"/>
+      <c r="B132" s="2" t="inlineStr">
+        <is>
+          <t>vangen</t>
+        </is>
+      </c>
+      <c r="C132" s="2" t="inlineStr">
+        <is>
+          <t>ving, vingen</t>
+        </is>
+      </c>
+      <c r="E132" s="2" t="inlineStr">
+        <is>
+          <t>gevangen</t>
+        </is>
+      </c>
+      <c r="F132" s="2" t="inlineStr">
+        <is>
+          <t>catch</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="133" s="3">
-      <c r="B133" s="2" t="n"/>
-      <c r="D133" s="2" t="n"/>
-      <c r="E133" s="2" t="n"/>
-      <c r="F133" s="2" t="n"/>
+      <c r="B133" s="2" t="inlineStr">
+        <is>
+          <t>varen</t>
+        </is>
+      </c>
+      <c r="C133" s="2" t="inlineStr">
+        <is>
+          <t>voer, voeren</t>
+        </is>
+      </c>
+      <c r="D133" s="2" t="inlineStr">
+        <is>
+          <t>(is)</t>
+        </is>
+      </c>
+      <c r="E133" s="2" t="inlineStr">
+        <is>
+          <t>gevaren</t>
+        </is>
+      </c>
+      <c r="F133" s="2" t="inlineStr">
+        <is>
+          <t>sail</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="134" s="3">
-      <c r="B134" s="2" t="n"/>
-      <c r="E134" s="2" t="n"/>
-      <c r="F134" s="2" t="n"/>
+      <c r="B134" s="2" t="inlineStr">
+        <is>
+          <t>vechten</t>
+        </is>
+      </c>
+      <c r="C134" s="2" t="inlineStr">
+        <is>
+          <t>vocht, vochten</t>
+        </is>
+      </c>
+      <c r="E134" s="2" t="inlineStr">
+        <is>
+          <t>gevochten</t>
+        </is>
+      </c>
+      <c r="F134" s="2" t="inlineStr">
+        <is>
+          <t>fight</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="135" s="3">
-      <c r="B135" s="2" t="n"/>
-      <c r="E135" s="2" t="n"/>
-      <c r="F135" s="2" t="n"/>
+      <c r="B135" s="2" t="inlineStr">
+        <is>
+          <t>verbieden</t>
+        </is>
+      </c>
+      <c r="C135" s="2" t="inlineStr">
+        <is>
+          <t>verbood, verboden</t>
+        </is>
+      </c>
+      <c r="E135" s="2" t="inlineStr">
+        <is>
+          <t>verboden</t>
+        </is>
+      </c>
+      <c r="F135" s="2" t="inlineStr">
+        <is>
+          <t>forbid</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="136" s="3">
-      <c r="B136" s="2" t="n"/>
-      <c r="D136" s="2" t="n"/>
-      <c r="E136" s="2" t="n"/>
-      <c r="F136" s="2" t="n"/>
+      <c r="B136" s="2" t="inlineStr">
+        <is>
+          <t>verdwijnen</t>
+        </is>
+      </c>
+      <c r="C136" s="2" t="inlineStr">
+        <is>
+          <t>verdween, verdwenen</t>
+        </is>
+      </c>
+      <c r="D136" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E136" s="2" t="inlineStr">
+        <is>
+          <t>verdwenen</t>
+        </is>
+      </c>
+      <c r="F136" s="2" t="inlineStr">
+        <is>
+          <t>disappear</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="137" s="3">
-      <c r="B137" s="2" t="n"/>
-      <c r="D137" s="2" t="n"/>
-      <c r="E137" s="2" t="n"/>
-      <c r="F137" s="2" t="n"/>
+      <c r="B137" s="2" t="inlineStr">
+        <is>
+          <t>vergeten</t>
+        </is>
+      </c>
+      <c r="C137" s="2" t="inlineStr">
+        <is>
+          <t>vergat, vergaten</t>
+        </is>
+      </c>
+      <c r="D137" s="2" t="inlineStr">
+        <is>
+          <t>(is)</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="inlineStr">
+        <is>
+          <t>vergeten</t>
+        </is>
+      </c>
+      <c r="F137" s="2" t="inlineStr">
+        <is>
+          <t>forget</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="138" s="3">
-      <c r="B138" s="2" t="n"/>
-      <c r="E138" s="2" t="n"/>
-      <c r="F138" s="2" t="n"/>
+      <c r="B138" s="2" t="inlineStr">
+        <is>
+          <t>verliezen</t>
+        </is>
+      </c>
+      <c r="C138" s="2" t="inlineStr">
+        <is>
+          <t>verloor, verloren</t>
+        </is>
+      </c>
+      <c r="E138" s="2" t="inlineStr">
+        <is>
+          <t>verloren</t>
+        </is>
+      </c>
+      <c r="F138" s="2" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="139" s="3">
-      <c r="B139" s="2" t="n"/>
-      <c r="E139" s="2" t="n"/>
-      <c r="F139" s="2" t="n"/>
+      <c r="B139" s="2" t="inlineStr">
+        <is>
+          <t>vermijden</t>
+        </is>
+      </c>
+      <c r="C139" s="2" t="inlineStr">
+        <is>
+          <t>vermeed, vermeden</t>
+        </is>
+      </c>
+      <c r="E139" s="2" t="inlineStr">
+        <is>
+          <t>vermeden</t>
+        </is>
+      </c>
+      <c r="F139" s="2" t="inlineStr">
+        <is>
+          <t>avoid</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="140" s="3">
-      <c r="B140" s="2" t="n"/>
-      <c r="E140" s="2" t="n"/>
-      <c r="F140" s="2" t="n"/>
+      <c r="B140" s="2" t="inlineStr">
+        <is>
+          <t>vinden</t>
+        </is>
+      </c>
+      <c r="C140" s="2" t="inlineStr">
+        <is>
+          <t>vond, vonden</t>
+        </is>
+      </c>
+      <c r="E140" s="2" t="inlineStr">
+        <is>
+          <t>gevonden</t>
+        </is>
+      </c>
+      <c r="F140" s="2" t="inlineStr">
+        <is>
+          <t>find</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="141" s="3">
-      <c r="B141" s="2" t="n"/>
-      <c r="E141" s="2" t="n"/>
-      <c r="F141" s="2" t="n"/>
+      <c r="B141" s="2" t="inlineStr">
+        <is>
+          <t>vliegen</t>
+        </is>
+      </c>
+      <c r="C141" s="2" t="inlineStr">
+        <is>
+          <t>vloog, vlogen</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="inlineStr">
+        <is>
+          <t>geviogen</t>
+        </is>
+      </c>
+      <c r="F141" s="2" t="inlineStr">
+        <is>
+          <t>fly</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="142" s="3">
-      <c r="B142" s="2" t="n"/>
-      <c r="E142" s="2" t="n"/>
-      <c r="F142" s="2" t="n"/>
+      <c r="B142" s="2" t="inlineStr">
+        <is>
+          <t>vouwen</t>
+        </is>
+      </c>
+      <c r="C142" s="2" t="inlineStr">
+        <is>
+          <t>vouwde, vouwden</t>
+        </is>
+      </c>
+      <c r="E142" s="2" t="inlineStr">
+        <is>
+          <t>gevouwen</t>
+        </is>
+      </c>
+      <c r="F142" s="2" t="inlineStr">
+        <is>
+          <t>fold</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="143" s="3">
-      <c r="B143" s="2" t="n"/>
-      <c r="E143" s="2" t="n"/>
-      <c r="F143" s="2" t="n"/>
+      <c r="B143" s="2" t="inlineStr">
+        <is>
+          <t>vragen</t>
+        </is>
+      </c>
+      <c r="C143" s="2" t="inlineStr">
+        <is>
+          <t>vroeg, vroegen</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="inlineStr">
+        <is>
+          <t>gevraagd</t>
+        </is>
+      </c>
+      <c r="F143" s="2" t="inlineStr">
+        <is>
+          <t>ask</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="144" s="3">
-      <c r="B144" s="2" t="n"/>
-      <c r="E144" s="2" t="n"/>
-      <c r="F144" s="2" t="n"/>
+      <c r="B144" s="2" t="inlineStr">
+        <is>
+          <t>vriezen</t>
+        </is>
+      </c>
+      <c r="C144" s="2" t="inlineStr">
+        <is>
+          <t>vroor, vroren</t>
+        </is>
+      </c>
+      <c r="E144" s="2" t="inlineStr">
+        <is>
+          <t>gevroren</t>
+        </is>
+      </c>
+      <c r="F144" s="2" t="inlineStr">
+        <is>
+          <t>freeze</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="145" s="3">
-      <c r="B145" s="2" t="n"/>
-      <c r="E145" s="2" t="n"/>
-      <c r="F145" s="2" t="n"/>
+      <c r="B145" s="2" t="inlineStr">
+        <is>
+          <t>waaien</t>
+        </is>
+      </c>
+      <c r="C145" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">waaide, waaiden, woei, woeien </t>
+        </is>
+      </c>
+      <c r="E145" s="2" t="inlineStr">
+        <is>
+          <t>gewaaid</t>
+        </is>
+      </c>
+      <c r="F145" s="2" t="inlineStr">
+        <is>
+          <t>blow</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="146" s="3">
-      <c r="B146" s="2" t="n"/>
-      <c r="E146" s="2" t="n"/>
-      <c r="F146" s="2" t="n"/>
+      <c r="B146" s="2" t="inlineStr">
+        <is>
+          <t>wassen</t>
+        </is>
+      </c>
+      <c r="C146" s="2" t="inlineStr">
+        <is>
+          <t>waste, wasten</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="inlineStr">
+        <is>
+          <t>gewassen</t>
+        </is>
+      </c>
+      <c r="F146" s="2" t="inlineStr">
+        <is>
+          <t>wash</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="147" s="3">
-      <c r="B147" s="2" t="n"/>
-      <c r="E147" s="2" t="n"/>
-      <c r="F147" s="2" t="n"/>
+      <c r="B147" s="2" t="inlineStr">
+        <is>
+          <t>wegen</t>
+        </is>
+      </c>
+      <c r="C147" s="2" t="inlineStr">
+        <is>
+          <t>woog, wogen</t>
+        </is>
+      </c>
+      <c r="E147" s="2" t="inlineStr">
+        <is>
+          <t>gewogen</t>
+        </is>
+      </c>
+      <c r="F147" s="2" t="inlineStr">
+        <is>
+          <t>weigh</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="148" s="3">
-      <c r="B148" s="2" t="n"/>
-      <c r="E148" s="2" t="n"/>
-      <c r="F148" s="2" t="n"/>
+      <c r="B148" s="2" t="inlineStr">
+        <is>
+          <t>werpen</t>
+        </is>
+      </c>
+      <c r="C148" s="2" t="inlineStr">
+        <is>
+          <t>wierp, wierpen</t>
+        </is>
+      </c>
+      <c r="E148" s="2" t="inlineStr">
+        <is>
+          <t>geworpen</t>
+        </is>
+      </c>
+      <c r="F148" s="2" t="inlineStr">
+        <is>
+          <t>throw</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="149" s="3">
-      <c r="B149" s="2" t="n"/>
-      <c r="E149" s="2" t="n"/>
-      <c r="F149" s="2" t="n"/>
+      <c r="B149" s="2" t="inlineStr">
+        <is>
+          <t>weten</t>
+        </is>
+      </c>
+      <c r="C149" s="2" t="inlineStr">
+        <is>
+          <t>wist, wisten</t>
+        </is>
+      </c>
+      <c r="E149" s="2" t="inlineStr">
+        <is>
+          <t>geweten</t>
+        </is>
+      </c>
+      <c r="F149" s="2" t="inlineStr">
+        <is>
+          <t>know</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="150" s="3">
-      <c r="B150" s="2" t="n"/>
-      <c r="E150" s="2" t="n"/>
-      <c r="F150" s="2" t="n"/>
+      <c r="B150" s="2" t="inlineStr">
+        <is>
+          <t>wijzen</t>
+        </is>
+      </c>
+      <c r="C150" s="2" t="inlineStr">
+        <is>
+          <t>wees, wezen</t>
+        </is>
+      </c>
+      <c r="E150" s="2" t="inlineStr">
+        <is>
+          <t>gewezen</t>
+        </is>
+      </c>
+      <c r="F150" s="2" t="inlineStr">
+        <is>
+          <t>show, point</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="151" s="3">
-      <c r="B151" s="2" t="n"/>
-      <c r="E151" s="2" t="n"/>
-      <c r="F151" s="2" t="n"/>
+      <c r="B151" s="2" t="inlineStr">
+        <is>
+          <t>willen</t>
+        </is>
+      </c>
+      <c r="C151" s="2" t="inlineStr">
+        <is>
+          <t>wilde / wou, wilden</t>
+        </is>
+      </c>
+      <c r="E151" s="2" t="inlineStr">
+        <is>
+          <t>gewild</t>
+        </is>
+      </c>
+      <c r="F151" s="2" t="inlineStr">
+        <is>
+          <t>want</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="152" s="3">
-      <c r="B152" s="2" t="n"/>
-      <c r="E152" s="2" t="n"/>
-      <c r="F152" s="2" t="n"/>
+      <c r="B152" s="2" t="inlineStr">
+        <is>
+          <t>winnen</t>
+        </is>
+      </c>
+      <c r="C152" s="2" t="inlineStr">
+        <is>
+          <t>won, wonnen</t>
+        </is>
+      </c>
+      <c r="E152" s="2" t="inlineStr">
+        <is>
+          <t>gewonnen</t>
+        </is>
+      </c>
+      <c r="F152" s="2" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="153" s="3">
-      <c r="B153" s="2" t="n"/>
-      <c r="D153" s="2" t="n"/>
-      <c r="E153" s="2" t="n"/>
-      <c r="F153" s="2" t="n"/>
+      <c r="B153" s="2" t="inlineStr">
+        <is>
+          <t>worden</t>
+        </is>
+      </c>
+      <c r="C153" s="2" t="inlineStr">
+        <is>
+          <t>werd, werden</t>
+        </is>
+      </c>
+      <c r="D153" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E153" s="2" t="inlineStr">
+        <is>
+          <t>geworden</t>
+        </is>
+      </c>
+      <c r="F153" s="2" t="inlineStr">
+        <is>
+          <t>become</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="154" s="3">
-      <c r="B154" s="2" t="n"/>
-      <c r="E154" s="2" t="n"/>
-      <c r="F154" s="2" t="n"/>
+      <c r="B154" s="2" t="inlineStr">
+        <is>
+          <t>wrijven</t>
+        </is>
+      </c>
+      <c r="C154" s="2" t="inlineStr">
+        <is>
+          <t>wreef, wreven</t>
+        </is>
+      </c>
+      <c r="E154" s="2" t="inlineStr">
+        <is>
+          <t>gewreven</t>
+        </is>
+      </c>
+      <c r="F154" s="2" t="inlineStr">
+        <is>
+          <t>rub</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="155" s="3">
-      <c r="B155" s="2" t="n"/>
-      <c r="E155" s="2" t="n"/>
-      <c r="F155" s="2" t="n"/>
+      <c r="B155" s="2" t="inlineStr">
+        <is>
+          <t>zeggen</t>
+        </is>
+      </c>
+      <c r="C155" s="2" t="inlineStr">
+        <is>
+          <t>zei, zeiden</t>
+        </is>
+      </c>
+      <c r="E155" s="2" t="inlineStr">
+        <is>
+          <t>gezegd</t>
+        </is>
+      </c>
+      <c r="F155" s="2" t="inlineStr">
+        <is>
+          <t>say</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="156" s="3">
-      <c r="B156" s="2" t="n"/>
-      <c r="E156" s="2" t="n"/>
-      <c r="F156" s="2" t="n"/>
+      <c r="B156" s="2" t="inlineStr">
+        <is>
+          <t>zenden</t>
+        </is>
+      </c>
+      <c r="C156" s="2" t="inlineStr">
+        <is>
+          <t>zond, zonden</t>
+        </is>
+      </c>
+      <c r="E156" s="2" t="inlineStr">
+        <is>
+          <t>gezonden</t>
+        </is>
+      </c>
+      <c r="F156" s="2" t="inlineStr">
+        <is>
+          <t>send</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="157" s="3">
-      <c r="B157" s="2" t="n"/>
-      <c r="E157" s="2" t="n"/>
-      <c r="F157" s="2" t="n"/>
+      <c r="B157" s="2" t="inlineStr">
+        <is>
+          <t>zien</t>
+        </is>
+      </c>
+      <c r="C157" s="2" t="inlineStr">
+        <is>
+          <t>zag, zagen</t>
+        </is>
+      </c>
+      <c r="E157" s="2" t="inlineStr">
+        <is>
+          <t>gezien</t>
+        </is>
+      </c>
+      <c r="F157" s="2" t="inlineStr">
+        <is>
+          <t>see</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="158" s="3">
-      <c r="B158" s="2" t="n"/>
-      <c r="D158" s="2" t="n"/>
-      <c r="E158" s="2" t="n"/>
-      <c r="F158" s="2" t="n"/>
+      <c r="B158" s="2" t="inlineStr">
+        <is>
+          <t>zijn</t>
+        </is>
+      </c>
+      <c r="C158" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">was, waren </t>
+        </is>
+      </c>
+      <c r="D158" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E158" s="2" t="inlineStr">
+        <is>
+          <t>geweest</t>
+        </is>
+      </c>
+      <c r="F158" s="2" t="inlineStr">
+        <is>
+          <t>be</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="159" s="3">
-      <c r="B159" s="2" t="n"/>
-      <c r="E159" s="2" t="n"/>
-      <c r="F159" s="2" t="n"/>
+      <c r="B159" s="2" t="inlineStr">
+        <is>
+          <t>zingen</t>
+        </is>
+      </c>
+      <c r="C159" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">zong, zongen </t>
+        </is>
+      </c>
+      <c r="E159" s="2" t="inlineStr">
+        <is>
+          <t>gezongen</t>
+        </is>
+      </c>
+      <c r="F159" s="2" t="inlineStr">
+        <is>
+          <t>sing</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="160" s="3">
-      <c r="B160" s="2" t="n"/>
-      <c r="D160" s="2" t="n"/>
-      <c r="E160" s="2" t="n"/>
-      <c r="F160" s="2" t="n"/>
+      <c r="B160" s="2" t="inlineStr">
+        <is>
+          <t>zinken</t>
+        </is>
+      </c>
+      <c r="C160" s="2" t="inlineStr">
+        <is>
+          <t>zonk, zonken</t>
+        </is>
+      </c>
+      <c r="D160" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E160" s="2" t="inlineStr">
+        <is>
+          <t>gezonken</t>
+        </is>
+      </c>
+      <c r="F160" s="2" t="inlineStr">
+        <is>
+          <t>sink</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="161" s="3">
-      <c r="B161" s="2" t="n"/>
-      <c r="E161" s="2" t="n"/>
-      <c r="F161" s="2" t="n"/>
+      <c r="B161" s="2" t="inlineStr">
+        <is>
+          <t>zitten</t>
+        </is>
+      </c>
+      <c r="C161" s="2" t="inlineStr">
+        <is>
+          <t>zat, zaten</t>
+        </is>
+      </c>
+      <c r="E161" s="2" t="inlineStr">
+        <is>
+          <t>gezeten</t>
+        </is>
+      </c>
+      <c r="F161" s="2" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="162" s="3">
-      <c r="B162" s="2" t="n"/>
-      <c r="E162" s="2" t="n"/>
-      <c r="F162" s="2" t="n"/>
+      <c r="B162" s="2" t="inlineStr">
+        <is>
+          <t>zoeken</t>
+        </is>
+      </c>
+      <c r="C162" s="2" t="inlineStr">
+        <is>
+          <t>zocht, zochten</t>
+        </is>
+      </c>
+      <c r="E162" s="2" t="inlineStr">
+        <is>
+          <t>gezocht</t>
+        </is>
+      </c>
+      <c r="F162" s="2" t="inlineStr">
+        <is>
+          <t>search, look</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="163" s="3">
-      <c r="B163" s="2" t="n"/>
-      <c r="E163" s="2" t="n"/>
-      <c r="F163" s="2" t="n"/>
+      <c r="B163" s="2" t="inlineStr">
+        <is>
+          <t>zullen</t>
+        </is>
+      </c>
+      <c r="C163" s="2" t="inlineStr">
+        <is>
+          <t>zou, zouden</t>
+        </is>
+      </c>
+      <c r="E163" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F163" s="2" t="inlineStr">
+        <is>
+          <t>will, would</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="164" s="3">
-      <c r="B164" s="2" t="n"/>
-      <c r="D164" s="2" t="n"/>
-      <c r="E164" s="2" t="n"/>
-      <c r="F164" s="2" t="n"/>
+      <c r="B164" s="2" t="inlineStr">
+        <is>
+          <t>zwemmen</t>
+        </is>
+      </c>
+      <c r="C164" s="2" t="inlineStr">
+        <is>
+          <t>zwom, zwommen</t>
+        </is>
+      </c>
+      <c r="D164" s="2" t="inlineStr">
+        <is>
+          <t>(is)</t>
+        </is>
+      </c>
+      <c r="E164" s="2" t="inlineStr">
+        <is>
+          <t>gezwommen</t>
+        </is>
+      </c>
+      <c r="F164" s="2" t="inlineStr">
+        <is>
+          <t>swim</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="165" s="3">
-      <c r="B165" s="2" t="n"/>
-      <c r="D165" s="2" t="n"/>
-      <c r="E165" s="2" t="n"/>
-      <c r="F165" s="2" t="n"/>
+      <c r="B165" s="2" t="inlineStr">
+        <is>
+          <t>zweren</t>
+        </is>
+      </c>
+      <c r="C165" s="4" t="inlineStr">
+        <is>
+          <t>zwoer, zwoeren</t>
+        </is>
+      </c>
+      <c r="D165" s="4" t="n"/>
+      <c r="E165" s="2" t="inlineStr">
+        <is>
+          <t>gezworen</t>
+        </is>
+      </c>
+      <c r="F165" s="2" t="inlineStr">
+        <is>
+          <t>swear</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="166" s="3">
-      <c r="B166" s="2" t="n"/>
-      <c r="E166" s="2" t="n"/>
-      <c r="F166" s="2" t="n"/>
+      <c r="B166" s="2" t="inlineStr">
+        <is>
+          <t>zwijgen</t>
+        </is>
+      </c>
+      <c r="C166" s="2" t="inlineStr">
+        <is>
+          <t>zweeg, zwegen</t>
+        </is>
+      </c>
+      <c r="E166" s="2" t="inlineStr">
+        <is>
+          <t>gezwegen</t>
+        </is>
+      </c>
+      <c r="F166" s="2" t="inlineStr">
+        <is>
+          <t>be silent</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
@@ -3703,12 +4504,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A27" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="B123:C123 A2"/>
+      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="B139:F166 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="2" width="15.8"/>
+    <col customWidth="1" max="2" min="2" style="2" width="15.79"/>
     <col customWidth="1" max="5" min="5" style="2" width="14.76"/>
   </cols>
   <sheetData>
@@ -4448,10 +5249,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A12" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="1" pane="topLeft" sqref="B123:C123 A12"/>
+      <selection activeCell="A12" activeCellId="1" pane="topLeft" sqref="B139:F166 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="15.48"/>
   </cols>
@@ -5050,10 +5851,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="17.06"/>
   </cols>
@@ -5312,12 +6113,12 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A36" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="2" width="25.21"/>
+    <col customWidth="1" max="2" min="2" style="2" width="25.22"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="3">
@@ -6291,10 +7092,10 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A30" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="20.74"/>
     <col customWidth="1" max="5" min="5" style="2" width="17.54"/>
@@ -7308,10 +8109,10 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A19" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="27.65"/>
   </cols>
@@ -7914,12 +8715,12 @@
           <t>zweren</t>
         </is>
       </c>
-      <c r="B27" s="2" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>zwoer, zwoeren</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n"/>
+      <c r="C27" s="4" t="n"/>
       <c r="D27" s="2" t="inlineStr">
         <is>
           <t>gezworen</t>

</xml_diff>

<commit_message>
Revert "FInishing for first demo"
This reverts commit 8b56e32069b318ee907122f50339537f669e7542.
</commit_message>
<xml_diff>
--- a/Werkwoorden_Lijst.xlsx
+++ b/Werkwoorden_Lijst.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -43,11 +43,6 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -78,20 +73,17 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -395,13 +387,13 @@
   </sheetPr>
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="B139" activeCellId="0" pane="topLeft" sqref="B139:F166"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A118" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
+      <selection activeCell="B123" activeCellId="0" pane="topLeft" sqref="B123:C123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="3" min="3" style="2" width="15.91"/>
+    <col customWidth="1" max="3" min="3" style="2" width="24.68"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="3">
@@ -593,11 +585,7 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="8" s="3">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>doe</t>
-        </is>
-      </c>
+      <c r="A8" s="2" t="inlineStr"/>
       <c r="B8" s="2" t="inlineStr">
         <is>
           <t>doen</t>
@@ -3457,1028 +3445,239 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="123" s="3">
-      <c r="B123" s="2" t="inlineStr">
-        <is>
-          <t>staan</t>
-        </is>
-      </c>
-      <c r="C123" s="2" t="inlineStr">
-        <is>
-          <t>stond, stonden</t>
-        </is>
-      </c>
-      <c r="E123" s="2" t="inlineStr">
-        <is>
-          <t>gestaan</t>
-        </is>
-      </c>
-      <c r="F123" s="2" t="inlineStr">
-        <is>
-          <t>stand</t>
-        </is>
-      </c>
+      <c r="A123" s="2" t="inlineStr"/>
+      <c r="B123" s="2" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" s="2" t="inlineStr"/>
+      <c r="E123" s="2" t="inlineStr"/>
+      <c r="F123" s="2" t="inlineStr"/>
     </row>
     <row customHeight="1" ht="12.8" r="124" s="3">
-      <c r="B124" s="2" t="inlineStr">
-        <is>
-          <t>steken</t>
-        </is>
-      </c>
-      <c r="C124" s="2" t="inlineStr">
-        <is>
-          <t>stak, staken</t>
-        </is>
-      </c>
-      <c r="E124" s="2" t="inlineStr">
-        <is>
-          <t>gestoken</t>
-        </is>
-      </c>
-      <c r="F124" s="2" t="inlineStr">
-        <is>
-          <t>stab, sting</t>
-        </is>
-      </c>
+      <c r="B124" s="2" t="n"/>
+      <c r="E124" s="2" t="n"/>
+      <c r="F124" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="125" s="3">
-      <c r="B125" s="2" t="inlineStr">
-        <is>
-          <t>stelen</t>
-        </is>
-      </c>
-      <c r="C125" s="2" t="inlineStr">
-        <is>
-          <t>stal, stalen</t>
-        </is>
-      </c>
-      <c r="E125" s="2" t="inlineStr">
-        <is>
-          <t>gestolen</t>
-        </is>
-      </c>
-      <c r="F125" s="2" t="inlineStr">
-        <is>
-          <t>steal</t>
-        </is>
-      </c>
+      <c r="B125" s="2" t="n"/>
+      <c r="E125" s="2" t="n"/>
+      <c r="F125" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="126" s="3">
-      <c r="B126" s="2" t="inlineStr">
-        <is>
-          <t>sterven</t>
-        </is>
-      </c>
-      <c r="C126" s="2" t="inlineStr">
-        <is>
-          <t>stierf, stierven</t>
-        </is>
-      </c>
-      <c r="D126" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E126" s="2" t="inlineStr">
-        <is>
-          <t>gestorven</t>
-        </is>
-      </c>
-      <c r="F126" s="2" t="inlineStr">
-        <is>
-          <t>die</t>
-        </is>
-      </c>
+      <c r="B126" s="2" t="n"/>
+      <c r="D126" s="2" t="n"/>
+      <c r="E126" s="2" t="n"/>
+      <c r="F126" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="127" s="3">
-      <c r="B127" s="2" t="inlineStr">
-        <is>
-          <t>stijgen</t>
-        </is>
-      </c>
-      <c r="C127" s="2" t="inlineStr">
-        <is>
-          <t>steeg, stegen</t>
-        </is>
-      </c>
-      <c r="D127" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E127" s="2" t="inlineStr">
-        <is>
-          <t>isgestegen</t>
-        </is>
-      </c>
-      <c r="F127" s="2" t="inlineStr">
-        <is>
-          <t>climb</t>
-        </is>
-      </c>
+      <c r="B127" s="2" t="n"/>
+      <c r="D127" s="2" t="n"/>
+      <c r="E127" s="2" t="n"/>
+      <c r="F127" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="128" s="3">
-      <c r="B128" s="2" t="inlineStr">
-        <is>
-          <t>treden</t>
-        </is>
-      </c>
-      <c r="C128" s="2" t="inlineStr">
-        <is>
-          <t>trad, traden</t>
-        </is>
-      </c>
-      <c r="D128" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E128" s="2" t="inlineStr">
-        <is>
-          <t>getreden</t>
-        </is>
-      </c>
-      <c r="F128" s="2" t="inlineStr">
-        <is>
-          <t>step</t>
-        </is>
-      </c>
+      <c r="B128" s="2" t="n"/>
+      <c r="D128" s="2" t="n"/>
+      <c r="E128" s="2" t="n"/>
+      <c r="F128" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="129" s="3">
-      <c r="B129" s="2" t="inlineStr">
-        <is>
-          <t>treffen</t>
-        </is>
-      </c>
-      <c r="C129" s="2" t="inlineStr">
-        <is>
-          <t>trof, troffen</t>
-        </is>
-      </c>
-      <c r="E129" s="2" t="inlineStr">
-        <is>
-          <t>getroffen</t>
-        </is>
-      </c>
-      <c r="F129" s="2" t="inlineStr">
-        <is>
-          <t>hit</t>
-        </is>
-      </c>
+      <c r="B129" s="2" t="n"/>
+      <c r="E129" s="2" t="n"/>
+      <c r="F129" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="130" s="3">
-      <c r="B130" s="2" t="inlineStr">
-        <is>
-          <t>trekken</t>
-        </is>
-      </c>
-      <c r="C130" s="2" t="inlineStr">
-        <is>
-          <t>trok, trokken</t>
-        </is>
-      </c>
-      <c r="E130" s="2" t="inlineStr">
-        <is>
-          <t>getrokken</t>
-        </is>
-      </c>
-      <c r="F130" s="2" t="inlineStr">
-        <is>
-          <t>pull</t>
-        </is>
-      </c>
+      <c r="B130" s="2" t="n"/>
+      <c r="E130" s="2" t="n"/>
+      <c r="F130" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="131" s="3">
-      <c r="B131" s="2" t="inlineStr">
-        <is>
-          <t>vallen</t>
-        </is>
-      </c>
-      <c r="C131" s="2" t="inlineStr">
-        <is>
-          <t>viel, vielen</t>
-        </is>
-      </c>
-      <c r="D131" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E131" s="2" t="inlineStr">
-        <is>
-          <t>gevallen</t>
-        </is>
-      </c>
-      <c r="F131" s="2" t="inlineStr">
-        <is>
-          <t>fall</t>
-        </is>
-      </c>
+      <c r="B131" s="2" t="n"/>
+      <c r="D131" s="2" t="n"/>
+      <c r="E131" s="2" t="n"/>
+      <c r="F131" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="132" s="3">
-      <c r="B132" s="2" t="inlineStr">
-        <is>
-          <t>vangen</t>
-        </is>
-      </c>
-      <c r="C132" s="2" t="inlineStr">
-        <is>
-          <t>ving, vingen</t>
-        </is>
-      </c>
-      <c r="E132" s="2" t="inlineStr">
-        <is>
-          <t>gevangen</t>
-        </is>
-      </c>
-      <c r="F132" s="2" t="inlineStr">
-        <is>
-          <t>catch</t>
-        </is>
-      </c>
+      <c r="B132" s="2" t="n"/>
+      <c r="E132" s="2" t="n"/>
+      <c r="F132" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="133" s="3">
-      <c r="B133" s="2" t="inlineStr">
-        <is>
-          <t>varen</t>
-        </is>
-      </c>
-      <c r="C133" s="2" t="inlineStr">
-        <is>
-          <t>voer, voeren</t>
-        </is>
-      </c>
-      <c r="D133" s="2" t="inlineStr">
-        <is>
-          <t>(is)</t>
-        </is>
-      </c>
-      <c r="E133" s="2" t="inlineStr">
-        <is>
-          <t>gevaren</t>
-        </is>
-      </c>
-      <c r="F133" s="2" t="inlineStr">
-        <is>
-          <t>sail</t>
-        </is>
-      </c>
+      <c r="B133" s="2" t="n"/>
+      <c r="D133" s="2" t="n"/>
+      <c r="E133" s="2" t="n"/>
+      <c r="F133" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="134" s="3">
-      <c r="B134" s="2" t="inlineStr">
-        <is>
-          <t>vechten</t>
-        </is>
-      </c>
-      <c r="C134" s="2" t="inlineStr">
-        <is>
-          <t>vocht, vochten</t>
-        </is>
-      </c>
-      <c r="E134" s="2" t="inlineStr">
-        <is>
-          <t>gevochten</t>
-        </is>
-      </c>
-      <c r="F134" s="2" t="inlineStr">
-        <is>
-          <t>fight</t>
-        </is>
-      </c>
+      <c r="B134" s="2" t="n"/>
+      <c r="E134" s="2" t="n"/>
+      <c r="F134" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="135" s="3">
-      <c r="B135" s="2" t="inlineStr">
-        <is>
-          <t>verbieden</t>
-        </is>
-      </c>
-      <c r="C135" s="2" t="inlineStr">
-        <is>
-          <t>verbood, verboden</t>
-        </is>
-      </c>
-      <c r="E135" s="2" t="inlineStr">
-        <is>
-          <t>verboden</t>
-        </is>
-      </c>
-      <c r="F135" s="2" t="inlineStr">
-        <is>
-          <t>forbid</t>
-        </is>
-      </c>
+      <c r="B135" s="2" t="n"/>
+      <c r="E135" s="2" t="n"/>
+      <c r="F135" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="136" s="3">
-      <c r="B136" s="2" t="inlineStr">
-        <is>
-          <t>verdwijnen</t>
-        </is>
-      </c>
-      <c r="C136" s="2" t="inlineStr">
-        <is>
-          <t>verdween, verdwenen</t>
-        </is>
-      </c>
-      <c r="D136" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E136" s="2" t="inlineStr">
-        <is>
-          <t>verdwenen</t>
-        </is>
-      </c>
-      <c r="F136" s="2" t="inlineStr">
-        <is>
-          <t>disappear</t>
-        </is>
-      </c>
+      <c r="B136" s="2" t="n"/>
+      <c r="D136" s="2" t="n"/>
+      <c r="E136" s="2" t="n"/>
+      <c r="F136" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="137" s="3">
-      <c r="B137" s="2" t="inlineStr">
-        <is>
-          <t>vergeten</t>
-        </is>
-      </c>
-      <c r="C137" s="2" t="inlineStr">
-        <is>
-          <t>vergat, vergaten</t>
-        </is>
-      </c>
-      <c r="D137" s="2" t="inlineStr">
-        <is>
-          <t>(is)</t>
-        </is>
-      </c>
-      <c r="E137" s="2" t="inlineStr">
-        <is>
-          <t>vergeten</t>
-        </is>
-      </c>
-      <c r="F137" s="2" t="inlineStr">
-        <is>
-          <t>forget</t>
-        </is>
-      </c>
+      <c r="B137" s="2" t="n"/>
+      <c r="D137" s="2" t="n"/>
+      <c r="E137" s="2" t="n"/>
+      <c r="F137" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="138" s="3">
-      <c r="B138" s="2" t="inlineStr">
-        <is>
-          <t>verliezen</t>
-        </is>
-      </c>
-      <c r="C138" s="2" t="inlineStr">
-        <is>
-          <t>verloor, verloren</t>
-        </is>
-      </c>
-      <c r="E138" s="2" t="inlineStr">
-        <is>
-          <t>verloren</t>
-        </is>
-      </c>
-      <c r="F138" s="2" t="inlineStr">
-        <is>
-          <t>lose</t>
-        </is>
-      </c>
+      <c r="B138" s="2" t="n"/>
+      <c r="E138" s="2" t="n"/>
+      <c r="F138" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="139" s="3">
-      <c r="B139" s="2" t="inlineStr">
-        <is>
-          <t>vermijden</t>
-        </is>
-      </c>
-      <c r="C139" s="2" t="inlineStr">
-        <is>
-          <t>vermeed, vermeden</t>
-        </is>
-      </c>
-      <c r="E139" s="2" t="inlineStr">
-        <is>
-          <t>vermeden</t>
-        </is>
-      </c>
-      <c r="F139" s="2" t="inlineStr">
-        <is>
-          <t>avoid</t>
-        </is>
-      </c>
+      <c r="B139" s="2" t="n"/>
+      <c r="E139" s="2" t="n"/>
+      <c r="F139" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="140" s="3">
-      <c r="B140" s="2" t="inlineStr">
-        <is>
-          <t>vinden</t>
-        </is>
-      </c>
-      <c r="C140" s="2" t="inlineStr">
-        <is>
-          <t>vond, vonden</t>
-        </is>
-      </c>
-      <c r="E140" s="2" t="inlineStr">
-        <is>
-          <t>gevonden</t>
-        </is>
-      </c>
-      <c r="F140" s="2" t="inlineStr">
-        <is>
-          <t>find</t>
-        </is>
-      </c>
+      <c r="B140" s="2" t="n"/>
+      <c r="E140" s="2" t="n"/>
+      <c r="F140" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="141" s="3">
-      <c r="B141" s="2" t="inlineStr">
-        <is>
-          <t>vliegen</t>
-        </is>
-      </c>
-      <c r="C141" s="2" t="inlineStr">
-        <is>
-          <t>vloog, vlogen</t>
-        </is>
-      </c>
-      <c r="E141" s="2" t="inlineStr">
-        <is>
-          <t>geviogen</t>
-        </is>
-      </c>
-      <c r="F141" s="2" t="inlineStr">
-        <is>
-          <t>fly</t>
-        </is>
-      </c>
+      <c r="B141" s="2" t="n"/>
+      <c r="E141" s="2" t="n"/>
+      <c r="F141" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="142" s="3">
-      <c r="B142" s="2" t="inlineStr">
-        <is>
-          <t>vouwen</t>
-        </is>
-      </c>
-      <c r="C142" s="2" t="inlineStr">
-        <is>
-          <t>vouwde, vouwden</t>
-        </is>
-      </c>
-      <c r="E142" s="2" t="inlineStr">
-        <is>
-          <t>gevouwen</t>
-        </is>
-      </c>
-      <c r="F142" s="2" t="inlineStr">
-        <is>
-          <t>fold</t>
-        </is>
-      </c>
+      <c r="B142" s="2" t="n"/>
+      <c r="E142" s="2" t="n"/>
+      <c r="F142" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="143" s="3">
-      <c r="B143" s="2" t="inlineStr">
-        <is>
-          <t>vragen</t>
-        </is>
-      </c>
-      <c r="C143" s="2" t="inlineStr">
-        <is>
-          <t>vroeg, vroegen</t>
-        </is>
-      </c>
-      <c r="E143" s="2" t="inlineStr">
-        <is>
-          <t>gevraagd</t>
-        </is>
-      </c>
-      <c r="F143" s="2" t="inlineStr">
-        <is>
-          <t>ask</t>
-        </is>
-      </c>
+      <c r="B143" s="2" t="n"/>
+      <c r="E143" s="2" t="n"/>
+      <c r="F143" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="144" s="3">
-      <c r="B144" s="2" t="inlineStr">
-        <is>
-          <t>vriezen</t>
-        </is>
-      </c>
-      <c r="C144" s="2" t="inlineStr">
-        <is>
-          <t>vroor, vroren</t>
-        </is>
-      </c>
-      <c r="E144" s="2" t="inlineStr">
-        <is>
-          <t>gevroren</t>
-        </is>
-      </c>
-      <c r="F144" s="2" t="inlineStr">
-        <is>
-          <t>freeze</t>
-        </is>
-      </c>
+      <c r="B144" s="2" t="n"/>
+      <c r="E144" s="2" t="n"/>
+      <c r="F144" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="145" s="3">
-      <c r="B145" s="2" t="inlineStr">
-        <is>
-          <t>waaien</t>
-        </is>
-      </c>
-      <c r="C145" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">waaide, waaiden, woei, woeien </t>
-        </is>
-      </c>
-      <c r="E145" s="2" t="inlineStr">
-        <is>
-          <t>gewaaid</t>
-        </is>
-      </c>
-      <c r="F145" s="2" t="inlineStr">
-        <is>
-          <t>blow</t>
-        </is>
-      </c>
+      <c r="B145" s="2" t="n"/>
+      <c r="E145" s="2" t="n"/>
+      <c r="F145" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="146" s="3">
-      <c r="B146" s="2" t="inlineStr">
-        <is>
-          <t>wassen</t>
-        </is>
-      </c>
-      <c r="C146" s="2" t="inlineStr">
-        <is>
-          <t>waste, wasten</t>
-        </is>
-      </c>
-      <c r="E146" s="2" t="inlineStr">
-        <is>
-          <t>gewassen</t>
-        </is>
-      </c>
-      <c r="F146" s="2" t="inlineStr">
-        <is>
-          <t>wash</t>
-        </is>
-      </c>
+      <c r="B146" s="2" t="n"/>
+      <c r="E146" s="2" t="n"/>
+      <c r="F146" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="147" s="3">
-      <c r="B147" s="2" t="inlineStr">
-        <is>
-          <t>wegen</t>
-        </is>
-      </c>
-      <c r="C147" s="2" t="inlineStr">
-        <is>
-          <t>woog, wogen</t>
-        </is>
-      </c>
-      <c r="E147" s="2" t="inlineStr">
-        <is>
-          <t>gewogen</t>
-        </is>
-      </c>
-      <c r="F147" s="2" t="inlineStr">
-        <is>
-          <t>weigh</t>
-        </is>
-      </c>
+      <c r="B147" s="2" t="n"/>
+      <c r="E147" s="2" t="n"/>
+      <c r="F147" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="148" s="3">
-      <c r="B148" s="2" t="inlineStr">
-        <is>
-          <t>werpen</t>
-        </is>
-      </c>
-      <c r="C148" s="2" t="inlineStr">
-        <is>
-          <t>wierp, wierpen</t>
-        </is>
-      </c>
-      <c r="E148" s="2" t="inlineStr">
-        <is>
-          <t>geworpen</t>
-        </is>
-      </c>
-      <c r="F148" s="2" t="inlineStr">
-        <is>
-          <t>throw</t>
-        </is>
-      </c>
+      <c r="B148" s="2" t="n"/>
+      <c r="E148" s="2" t="n"/>
+      <c r="F148" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="149" s="3">
-      <c r="B149" s="2" t="inlineStr">
-        <is>
-          <t>weten</t>
-        </is>
-      </c>
-      <c r="C149" s="2" t="inlineStr">
-        <is>
-          <t>wist, wisten</t>
-        </is>
-      </c>
-      <c r="E149" s="2" t="inlineStr">
-        <is>
-          <t>geweten</t>
-        </is>
-      </c>
-      <c r="F149" s="2" t="inlineStr">
-        <is>
-          <t>know</t>
-        </is>
-      </c>
+      <c r="B149" s="2" t="n"/>
+      <c r="E149" s="2" t="n"/>
+      <c r="F149" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="150" s="3">
-      <c r="B150" s="2" t="inlineStr">
-        <is>
-          <t>wijzen</t>
-        </is>
-      </c>
-      <c r="C150" s="2" t="inlineStr">
-        <is>
-          <t>wees, wezen</t>
-        </is>
-      </c>
-      <c r="E150" s="2" t="inlineStr">
-        <is>
-          <t>gewezen</t>
-        </is>
-      </c>
-      <c r="F150" s="2" t="inlineStr">
-        <is>
-          <t>show, point</t>
-        </is>
-      </c>
+      <c r="B150" s="2" t="n"/>
+      <c r="E150" s="2" t="n"/>
+      <c r="F150" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="151" s="3">
-      <c r="B151" s="2" t="inlineStr">
-        <is>
-          <t>willen</t>
-        </is>
-      </c>
-      <c r="C151" s="2" t="inlineStr">
-        <is>
-          <t>wilde / wou, wilden</t>
-        </is>
-      </c>
-      <c r="E151" s="2" t="inlineStr">
-        <is>
-          <t>gewild</t>
-        </is>
-      </c>
-      <c r="F151" s="2" t="inlineStr">
-        <is>
-          <t>want</t>
-        </is>
-      </c>
+      <c r="B151" s="2" t="n"/>
+      <c r="E151" s="2" t="n"/>
+      <c r="F151" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="152" s="3">
-      <c r="B152" s="2" t="inlineStr">
-        <is>
-          <t>winnen</t>
-        </is>
-      </c>
-      <c r="C152" s="2" t="inlineStr">
-        <is>
-          <t>won, wonnen</t>
-        </is>
-      </c>
-      <c r="E152" s="2" t="inlineStr">
-        <is>
-          <t>gewonnen</t>
-        </is>
-      </c>
-      <c r="F152" s="2" t="inlineStr">
-        <is>
-          <t>win</t>
-        </is>
-      </c>
+      <c r="B152" s="2" t="n"/>
+      <c r="E152" s="2" t="n"/>
+      <c r="F152" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="153" s="3">
-      <c r="B153" s="2" t="inlineStr">
-        <is>
-          <t>worden</t>
-        </is>
-      </c>
-      <c r="C153" s="2" t="inlineStr">
-        <is>
-          <t>werd, werden</t>
-        </is>
-      </c>
-      <c r="D153" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E153" s="2" t="inlineStr">
-        <is>
-          <t>geworden</t>
-        </is>
-      </c>
-      <c r="F153" s="2" t="inlineStr">
-        <is>
-          <t>become</t>
-        </is>
-      </c>
+      <c r="B153" s="2" t="n"/>
+      <c r="D153" s="2" t="n"/>
+      <c r="E153" s="2" t="n"/>
+      <c r="F153" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="154" s="3">
-      <c r="B154" s="2" t="inlineStr">
-        <is>
-          <t>wrijven</t>
-        </is>
-      </c>
-      <c r="C154" s="2" t="inlineStr">
-        <is>
-          <t>wreef, wreven</t>
-        </is>
-      </c>
-      <c r="E154" s="2" t="inlineStr">
-        <is>
-          <t>gewreven</t>
-        </is>
-      </c>
-      <c r="F154" s="2" t="inlineStr">
-        <is>
-          <t>rub</t>
-        </is>
-      </c>
+      <c r="B154" s="2" t="n"/>
+      <c r="E154" s="2" t="n"/>
+      <c r="F154" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="155" s="3">
-      <c r="B155" s="2" t="inlineStr">
-        <is>
-          <t>zeggen</t>
-        </is>
-      </c>
-      <c r="C155" s="2" t="inlineStr">
-        <is>
-          <t>zei, zeiden</t>
-        </is>
-      </c>
-      <c r="E155" s="2" t="inlineStr">
-        <is>
-          <t>gezegd</t>
-        </is>
-      </c>
-      <c r="F155" s="2" t="inlineStr">
-        <is>
-          <t>say</t>
-        </is>
-      </c>
+      <c r="B155" s="2" t="n"/>
+      <c r="E155" s="2" t="n"/>
+      <c r="F155" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="156" s="3">
-      <c r="B156" s="2" t="inlineStr">
-        <is>
-          <t>zenden</t>
-        </is>
-      </c>
-      <c r="C156" s="2" t="inlineStr">
-        <is>
-          <t>zond, zonden</t>
-        </is>
-      </c>
-      <c r="E156" s="2" t="inlineStr">
-        <is>
-          <t>gezonden</t>
-        </is>
-      </c>
-      <c r="F156" s="2" t="inlineStr">
-        <is>
-          <t>send</t>
-        </is>
-      </c>
+      <c r="B156" s="2" t="n"/>
+      <c r="E156" s="2" t="n"/>
+      <c r="F156" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="157" s="3">
-      <c r="B157" s="2" t="inlineStr">
-        <is>
-          <t>zien</t>
-        </is>
-      </c>
-      <c r="C157" s="2" t="inlineStr">
-        <is>
-          <t>zag, zagen</t>
-        </is>
-      </c>
-      <c r="E157" s="2" t="inlineStr">
-        <is>
-          <t>gezien</t>
-        </is>
-      </c>
-      <c r="F157" s="2" t="inlineStr">
-        <is>
-          <t>see</t>
-        </is>
-      </c>
+      <c r="B157" s="2" t="n"/>
+      <c r="E157" s="2" t="n"/>
+      <c r="F157" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="158" s="3">
-      <c r="B158" s="2" t="inlineStr">
-        <is>
-          <t>zijn</t>
-        </is>
-      </c>
-      <c r="C158" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">was, waren </t>
-        </is>
-      </c>
-      <c r="D158" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E158" s="2" t="inlineStr">
-        <is>
-          <t>geweest</t>
-        </is>
-      </c>
-      <c r="F158" s="2" t="inlineStr">
-        <is>
-          <t>be</t>
-        </is>
-      </c>
+      <c r="B158" s="2" t="n"/>
+      <c r="D158" s="2" t="n"/>
+      <c r="E158" s="2" t="n"/>
+      <c r="F158" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="159" s="3">
-      <c r="B159" s="2" t="inlineStr">
-        <is>
-          <t>zingen</t>
-        </is>
-      </c>
-      <c r="C159" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">zong, zongen </t>
-        </is>
-      </c>
-      <c r="E159" s="2" t="inlineStr">
-        <is>
-          <t>gezongen</t>
-        </is>
-      </c>
-      <c r="F159" s="2" t="inlineStr">
-        <is>
-          <t>sing</t>
-        </is>
-      </c>
+      <c r="B159" s="2" t="n"/>
+      <c r="E159" s="2" t="n"/>
+      <c r="F159" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="160" s="3">
-      <c r="B160" s="2" t="inlineStr">
-        <is>
-          <t>zinken</t>
-        </is>
-      </c>
-      <c r="C160" s="2" t="inlineStr">
-        <is>
-          <t>zonk, zonken</t>
-        </is>
-      </c>
-      <c r="D160" s="2" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="E160" s="2" t="inlineStr">
-        <is>
-          <t>gezonken</t>
-        </is>
-      </c>
-      <c r="F160" s="2" t="inlineStr">
-        <is>
-          <t>sink</t>
-        </is>
-      </c>
+      <c r="B160" s="2" t="n"/>
+      <c r="D160" s="2" t="n"/>
+      <c r="E160" s="2" t="n"/>
+      <c r="F160" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="161" s="3">
-      <c r="B161" s="2" t="inlineStr">
-        <is>
-          <t>zitten</t>
-        </is>
-      </c>
-      <c r="C161" s="2" t="inlineStr">
-        <is>
-          <t>zat, zaten</t>
-        </is>
-      </c>
-      <c r="E161" s="2" t="inlineStr">
-        <is>
-          <t>gezeten</t>
-        </is>
-      </c>
-      <c r="F161" s="2" t="inlineStr">
-        <is>
-          <t>sit</t>
-        </is>
-      </c>
+      <c r="B161" s="2" t="n"/>
+      <c r="E161" s="2" t="n"/>
+      <c r="F161" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="162" s="3">
-      <c r="B162" s="2" t="inlineStr">
-        <is>
-          <t>zoeken</t>
-        </is>
-      </c>
-      <c r="C162" s="2" t="inlineStr">
-        <is>
-          <t>zocht, zochten</t>
-        </is>
-      </c>
-      <c r="E162" s="2" t="inlineStr">
-        <is>
-          <t>gezocht</t>
-        </is>
-      </c>
-      <c r="F162" s="2" t="inlineStr">
-        <is>
-          <t>search, look</t>
-        </is>
-      </c>
+      <c r="B162" s="2" t="n"/>
+      <c r="E162" s="2" t="n"/>
+      <c r="F162" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="163" s="3">
-      <c r="B163" s="2" t="inlineStr">
-        <is>
-          <t>zullen</t>
-        </is>
-      </c>
-      <c r="C163" s="2" t="inlineStr">
-        <is>
-          <t>zou, zouden</t>
-        </is>
-      </c>
-      <c r="E163" s="2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F163" s="2" t="inlineStr">
-        <is>
-          <t>will, would</t>
-        </is>
-      </c>
+      <c r="B163" s="2" t="n"/>
+      <c r="E163" s="2" t="n"/>
+      <c r="F163" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="164" s="3">
-      <c r="B164" s="2" t="inlineStr">
-        <is>
-          <t>zwemmen</t>
-        </is>
-      </c>
-      <c r="C164" s="2" t="inlineStr">
-        <is>
-          <t>zwom, zwommen</t>
-        </is>
-      </c>
-      <c r="D164" s="2" t="inlineStr">
-        <is>
-          <t>(is)</t>
-        </is>
-      </c>
-      <c r="E164" s="2" t="inlineStr">
-        <is>
-          <t>gezwommen</t>
-        </is>
-      </c>
-      <c r="F164" s="2" t="inlineStr">
-        <is>
-          <t>swim</t>
-        </is>
-      </c>
+      <c r="B164" s="2" t="n"/>
+      <c r="D164" s="2" t="n"/>
+      <c r="E164" s="2" t="n"/>
+      <c r="F164" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="165" s="3">
-      <c r="B165" s="2" t="inlineStr">
-        <is>
-          <t>zweren</t>
-        </is>
-      </c>
-      <c r="C165" s="4" t="inlineStr">
-        <is>
-          <t>zwoer, zwoeren</t>
-        </is>
-      </c>
-      <c r="D165" s="4" t="n"/>
-      <c r="E165" s="2" t="inlineStr">
-        <is>
-          <t>gezworen</t>
-        </is>
-      </c>
-      <c r="F165" s="2" t="inlineStr">
-        <is>
-          <t>swear</t>
-        </is>
-      </c>
+      <c r="B165" s="2" t="n"/>
+      <c r="D165" s="2" t="n"/>
+      <c r="E165" s="2" t="n"/>
+      <c r="F165" s="2" t="n"/>
     </row>
     <row customHeight="1" ht="12.8" r="166" s="3">
-      <c r="B166" s="2" t="inlineStr">
-        <is>
-          <t>zwijgen</t>
-        </is>
-      </c>
-      <c r="C166" s="2" t="inlineStr">
-        <is>
-          <t>zweeg, zwegen</t>
-        </is>
-      </c>
-      <c r="E166" s="2" t="inlineStr">
-        <is>
-          <t>gezwegen</t>
-        </is>
-      </c>
-      <c r="F166" s="2" t="inlineStr">
-        <is>
-          <t>be silent</t>
-        </is>
-      </c>
+      <c r="B166" s="2" t="n"/>
+      <c r="E166" s="2" t="n"/>
+      <c r="F166" s="2" t="n"/>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
@@ -4504,12 +3703,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A27" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="B139:F166 A2"/>
+      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="B123:C123 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="2" width="15.79"/>
+    <col customWidth="1" max="2" min="2" style="2" width="15.8"/>
     <col customWidth="1" max="5" min="5" style="2" width="14.76"/>
   </cols>
   <sheetData>
@@ -5249,10 +4448,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A12" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="1" pane="topLeft" sqref="B139:F166 A12"/>
+      <selection activeCell="A12" activeCellId="1" pane="topLeft" sqref="B123:C123 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="15.48"/>
   </cols>
@@ -5851,10 +5050,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="17.06"/>
   </cols>
@@ -6113,12 +5312,12 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A36" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="2" width="25.22"/>
+    <col customWidth="1" max="2" min="2" style="2" width="25.21"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="3">
@@ -7092,10 +6291,10 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A30" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="20.74"/>
     <col customWidth="1" max="5" min="5" style="2" width="17.54"/>
@@ -8109,10 +7308,10 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A19" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="27.65"/>
   </cols>
@@ -8715,12 +7914,12 @@
           <t>zweren</t>
         </is>
       </c>
-      <c r="B27" s="4" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>zwoer, zwoeren</t>
         </is>
       </c>
-      <c r="C27" s="4" t="n"/>
+      <c r="C27" s="2" t="n"/>
       <c r="D27" s="2" t="inlineStr">
         <is>
           <t>gezworen</t>

</xml_diff>

<commit_message>
Revert "Revert "FInishing for first demo""
This reverts commit 57b627578a89a0e88d8c7225d7fe7ac6dfb54309.
</commit_message>
<xml_diff>
--- a/Werkwoorden_Lijst.xlsx
+++ b/Werkwoorden_Lijst.xlsx
@@ -23,7 +23,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -43,6 +43,11 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -73,17 +78,20 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -387,13 +395,13 @@
   </sheetPr>
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A118" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="B123" activeCellId="0" pane="topLeft" sqref="B123:C123"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
+      <selection activeCell="B139" activeCellId="0" pane="topLeft" sqref="B139:F166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.60546875" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.55078125" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="3" min="3" style="2" width="24.68"/>
+    <col customWidth="1" max="3" min="3" style="2" width="15.91"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="3">
@@ -585,7 +593,11 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="8" s="3">
-      <c r="A8" s="2" t="inlineStr"/>
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>doe</t>
+        </is>
+      </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
           <t>doen</t>
@@ -3445,239 +3457,1028 @@
       </c>
     </row>
     <row customHeight="1" ht="12.8" r="123" s="3">
-      <c r="A123" s="2" t="inlineStr"/>
-      <c r="B123" s="2" t="inlineStr"/>
-      <c r="C123" t="inlineStr"/>
-      <c r="D123" s="2" t="inlineStr"/>
-      <c r="E123" s="2" t="inlineStr"/>
-      <c r="F123" s="2" t="inlineStr"/>
+      <c r="B123" s="2" t="inlineStr">
+        <is>
+          <t>staan</t>
+        </is>
+      </c>
+      <c r="C123" s="2" t="inlineStr">
+        <is>
+          <t>stond, stonden</t>
+        </is>
+      </c>
+      <c r="E123" s="2" t="inlineStr">
+        <is>
+          <t>gestaan</t>
+        </is>
+      </c>
+      <c r="F123" s="2" t="inlineStr">
+        <is>
+          <t>stand</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="124" s="3">
-      <c r="B124" s="2" t="n"/>
-      <c r="E124" s="2" t="n"/>
-      <c r="F124" s="2" t="n"/>
+      <c r="B124" s="2" t="inlineStr">
+        <is>
+          <t>steken</t>
+        </is>
+      </c>
+      <c r="C124" s="2" t="inlineStr">
+        <is>
+          <t>stak, staken</t>
+        </is>
+      </c>
+      <c r="E124" s="2" t="inlineStr">
+        <is>
+          <t>gestoken</t>
+        </is>
+      </c>
+      <c r="F124" s="2" t="inlineStr">
+        <is>
+          <t>stab, sting</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="125" s="3">
-      <c r="B125" s="2" t="n"/>
-      <c r="E125" s="2" t="n"/>
-      <c r="F125" s="2" t="n"/>
+      <c r="B125" s="2" t="inlineStr">
+        <is>
+          <t>stelen</t>
+        </is>
+      </c>
+      <c r="C125" s="2" t="inlineStr">
+        <is>
+          <t>stal, stalen</t>
+        </is>
+      </c>
+      <c r="E125" s="2" t="inlineStr">
+        <is>
+          <t>gestolen</t>
+        </is>
+      </c>
+      <c r="F125" s="2" t="inlineStr">
+        <is>
+          <t>steal</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="126" s="3">
-      <c r="B126" s="2" t="n"/>
-      <c r="D126" s="2" t="n"/>
-      <c r="E126" s="2" t="n"/>
-      <c r="F126" s="2" t="n"/>
+      <c r="B126" s="2" t="inlineStr">
+        <is>
+          <t>sterven</t>
+        </is>
+      </c>
+      <c r="C126" s="2" t="inlineStr">
+        <is>
+          <t>stierf, stierven</t>
+        </is>
+      </c>
+      <c r="D126" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E126" s="2" t="inlineStr">
+        <is>
+          <t>gestorven</t>
+        </is>
+      </c>
+      <c r="F126" s="2" t="inlineStr">
+        <is>
+          <t>die</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="127" s="3">
-      <c r="B127" s="2" t="n"/>
-      <c r="D127" s="2" t="n"/>
-      <c r="E127" s="2" t="n"/>
-      <c r="F127" s="2" t="n"/>
+      <c r="B127" s="2" t="inlineStr">
+        <is>
+          <t>stijgen</t>
+        </is>
+      </c>
+      <c r="C127" s="2" t="inlineStr">
+        <is>
+          <t>steeg, stegen</t>
+        </is>
+      </c>
+      <c r="D127" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E127" s="2" t="inlineStr">
+        <is>
+          <t>isgestegen</t>
+        </is>
+      </c>
+      <c r="F127" s="2" t="inlineStr">
+        <is>
+          <t>climb</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="128" s="3">
-      <c r="B128" s="2" t="n"/>
-      <c r="D128" s="2" t="n"/>
-      <c r="E128" s="2" t="n"/>
-      <c r="F128" s="2" t="n"/>
+      <c r="B128" s="2" t="inlineStr">
+        <is>
+          <t>treden</t>
+        </is>
+      </c>
+      <c r="C128" s="2" t="inlineStr">
+        <is>
+          <t>trad, traden</t>
+        </is>
+      </c>
+      <c r="D128" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E128" s="2" t="inlineStr">
+        <is>
+          <t>getreden</t>
+        </is>
+      </c>
+      <c r="F128" s="2" t="inlineStr">
+        <is>
+          <t>step</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="129" s="3">
-      <c r="B129" s="2" t="n"/>
-      <c r="E129" s="2" t="n"/>
-      <c r="F129" s="2" t="n"/>
+      <c r="B129" s="2" t="inlineStr">
+        <is>
+          <t>treffen</t>
+        </is>
+      </c>
+      <c r="C129" s="2" t="inlineStr">
+        <is>
+          <t>trof, troffen</t>
+        </is>
+      </c>
+      <c r="E129" s="2" t="inlineStr">
+        <is>
+          <t>getroffen</t>
+        </is>
+      </c>
+      <c r="F129" s="2" t="inlineStr">
+        <is>
+          <t>hit</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="130" s="3">
-      <c r="B130" s="2" t="n"/>
-      <c r="E130" s="2" t="n"/>
-      <c r="F130" s="2" t="n"/>
+      <c r="B130" s="2" t="inlineStr">
+        <is>
+          <t>trekken</t>
+        </is>
+      </c>
+      <c r="C130" s="2" t="inlineStr">
+        <is>
+          <t>trok, trokken</t>
+        </is>
+      </c>
+      <c r="E130" s="2" t="inlineStr">
+        <is>
+          <t>getrokken</t>
+        </is>
+      </c>
+      <c r="F130" s="2" t="inlineStr">
+        <is>
+          <t>pull</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="131" s="3">
-      <c r="B131" s="2" t="n"/>
-      <c r="D131" s="2" t="n"/>
-      <c r="E131" s="2" t="n"/>
-      <c r="F131" s="2" t="n"/>
+      <c r="B131" s="2" t="inlineStr">
+        <is>
+          <t>vallen</t>
+        </is>
+      </c>
+      <c r="C131" s="2" t="inlineStr">
+        <is>
+          <t>viel, vielen</t>
+        </is>
+      </c>
+      <c r="D131" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E131" s="2" t="inlineStr">
+        <is>
+          <t>gevallen</t>
+        </is>
+      </c>
+      <c r="F131" s="2" t="inlineStr">
+        <is>
+          <t>fall</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="132" s="3">
-      <c r="B132" s="2" t="n"/>
-      <c r="E132" s="2" t="n"/>
-      <c r="F132" s="2" t="n"/>
+      <c r="B132" s="2" t="inlineStr">
+        <is>
+          <t>vangen</t>
+        </is>
+      </c>
+      <c r="C132" s="2" t="inlineStr">
+        <is>
+          <t>ving, vingen</t>
+        </is>
+      </c>
+      <c r="E132" s="2" t="inlineStr">
+        <is>
+          <t>gevangen</t>
+        </is>
+      </c>
+      <c r="F132" s="2" t="inlineStr">
+        <is>
+          <t>catch</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="133" s="3">
-      <c r="B133" s="2" t="n"/>
-      <c r="D133" s="2" t="n"/>
-      <c r="E133" s="2" t="n"/>
-      <c r="F133" s="2" t="n"/>
+      <c r="B133" s="2" t="inlineStr">
+        <is>
+          <t>varen</t>
+        </is>
+      </c>
+      <c r="C133" s="2" t="inlineStr">
+        <is>
+          <t>voer, voeren</t>
+        </is>
+      </c>
+      <c r="D133" s="2" t="inlineStr">
+        <is>
+          <t>(is)</t>
+        </is>
+      </c>
+      <c r="E133" s="2" t="inlineStr">
+        <is>
+          <t>gevaren</t>
+        </is>
+      </c>
+      <c r="F133" s="2" t="inlineStr">
+        <is>
+          <t>sail</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="134" s="3">
-      <c r="B134" s="2" t="n"/>
-      <c r="E134" s="2" t="n"/>
-      <c r="F134" s="2" t="n"/>
+      <c r="B134" s="2" t="inlineStr">
+        <is>
+          <t>vechten</t>
+        </is>
+      </c>
+      <c r="C134" s="2" t="inlineStr">
+        <is>
+          <t>vocht, vochten</t>
+        </is>
+      </c>
+      <c r="E134" s="2" t="inlineStr">
+        <is>
+          <t>gevochten</t>
+        </is>
+      </c>
+      <c r="F134" s="2" t="inlineStr">
+        <is>
+          <t>fight</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="135" s="3">
-      <c r="B135" s="2" t="n"/>
-      <c r="E135" s="2" t="n"/>
-      <c r="F135" s="2" t="n"/>
+      <c r="B135" s="2" t="inlineStr">
+        <is>
+          <t>verbieden</t>
+        </is>
+      </c>
+      <c r="C135" s="2" t="inlineStr">
+        <is>
+          <t>verbood, verboden</t>
+        </is>
+      </c>
+      <c r="E135" s="2" t="inlineStr">
+        <is>
+          <t>verboden</t>
+        </is>
+      </c>
+      <c r="F135" s="2" t="inlineStr">
+        <is>
+          <t>forbid</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="136" s="3">
-      <c r="B136" s="2" t="n"/>
-      <c r="D136" s="2" t="n"/>
-      <c r="E136" s="2" t="n"/>
-      <c r="F136" s="2" t="n"/>
+      <c r="B136" s="2" t="inlineStr">
+        <is>
+          <t>verdwijnen</t>
+        </is>
+      </c>
+      <c r="C136" s="2" t="inlineStr">
+        <is>
+          <t>verdween, verdwenen</t>
+        </is>
+      </c>
+      <c r="D136" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E136" s="2" t="inlineStr">
+        <is>
+          <t>verdwenen</t>
+        </is>
+      </c>
+      <c r="F136" s="2" t="inlineStr">
+        <is>
+          <t>disappear</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="137" s="3">
-      <c r="B137" s="2" t="n"/>
-      <c r="D137" s="2" t="n"/>
-      <c r="E137" s="2" t="n"/>
-      <c r="F137" s="2" t="n"/>
+      <c r="B137" s="2" t="inlineStr">
+        <is>
+          <t>vergeten</t>
+        </is>
+      </c>
+      <c r="C137" s="2" t="inlineStr">
+        <is>
+          <t>vergat, vergaten</t>
+        </is>
+      </c>
+      <c r="D137" s="2" t="inlineStr">
+        <is>
+          <t>(is)</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="inlineStr">
+        <is>
+          <t>vergeten</t>
+        </is>
+      </c>
+      <c r="F137" s="2" t="inlineStr">
+        <is>
+          <t>forget</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="138" s="3">
-      <c r="B138" s="2" t="n"/>
-      <c r="E138" s="2" t="n"/>
-      <c r="F138" s="2" t="n"/>
+      <c r="B138" s="2" t="inlineStr">
+        <is>
+          <t>verliezen</t>
+        </is>
+      </c>
+      <c r="C138" s="2" t="inlineStr">
+        <is>
+          <t>verloor, verloren</t>
+        </is>
+      </c>
+      <c r="E138" s="2" t="inlineStr">
+        <is>
+          <t>verloren</t>
+        </is>
+      </c>
+      <c r="F138" s="2" t="inlineStr">
+        <is>
+          <t>lose</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="139" s="3">
-      <c r="B139" s="2" t="n"/>
-      <c r="E139" s="2" t="n"/>
-      <c r="F139" s="2" t="n"/>
+      <c r="B139" s="2" t="inlineStr">
+        <is>
+          <t>vermijden</t>
+        </is>
+      </c>
+      <c r="C139" s="2" t="inlineStr">
+        <is>
+          <t>vermeed, vermeden</t>
+        </is>
+      </c>
+      <c r="E139" s="2" t="inlineStr">
+        <is>
+          <t>vermeden</t>
+        </is>
+      </c>
+      <c r="F139" s="2" t="inlineStr">
+        <is>
+          <t>avoid</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="140" s="3">
-      <c r="B140" s="2" t="n"/>
-      <c r="E140" s="2" t="n"/>
-      <c r="F140" s="2" t="n"/>
+      <c r="B140" s="2" t="inlineStr">
+        <is>
+          <t>vinden</t>
+        </is>
+      </c>
+      <c r="C140" s="2" t="inlineStr">
+        <is>
+          <t>vond, vonden</t>
+        </is>
+      </c>
+      <c r="E140" s="2" t="inlineStr">
+        <is>
+          <t>gevonden</t>
+        </is>
+      </c>
+      <c r="F140" s="2" t="inlineStr">
+        <is>
+          <t>find</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="141" s="3">
-      <c r="B141" s="2" t="n"/>
-      <c r="E141" s="2" t="n"/>
-      <c r="F141" s="2" t="n"/>
+      <c r="B141" s="2" t="inlineStr">
+        <is>
+          <t>vliegen</t>
+        </is>
+      </c>
+      <c r="C141" s="2" t="inlineStr">
+        <is>
+          <t>vloog, vlogen</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="inlineStr">
+        <is>
+          <t>geviogen</t>
+        </is>
+      </c>
+      <c r="F141" s="2" t="inlineStr">
+        <is>
+          <t>fly</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="142" s="3">
-      <c r="B142" s="2" t="n"/>
-      <c r="E142" s="2" t="n"/>
-      <c r="F142" s="2" t="n"/>
+      <c r="B142" s="2" t="inlineStr">
+        <is>
+          <t>vouwen</t>
+        </is>
+      </c>
+      <c r="C142" s="2" t="inlineStr">
+        <is>
+          <t>vouwde, vouwden</t>
+        </is>
+      </c>
+      <c r="E142" s="2" t="inlineStr">
+        <is>
+          <t>gevouwen</t>
+        </is>
+      </c>
+      <c r="F142" s="2" t="inlineStr">
+        <is>
+          <t>fold</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="143" s="3">
-      <c r="B143" s="2" t="n"/>
-      <c r="E143" s="2" t="n"/>
-      <c r="F143" s="2" t="n"/>
+      <c r="B143" s="2" t="inlineStr">
+        <is>
+          <t>vragen</t>
+        </is>
+      </c>
+      <c r="C143" s="2" t="inlineStr">
+        <is>
+          <t>vroeg, vroegen</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="inlineStr">
+        <is>
+          <t>gevraagd</t>
+        </is>
+      </c>
+      <c r="F143" s="2" t="inlineStr">
+        <is>
+          <t>ask</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="144" s="3">
-      <c r="B144" s="2" t="n"/>
-      <c r="E144" s="2" t="n"/>
-      <c r="F144" s="2" t="n"/>
+      <c r="B144" s="2" t="inlineStr">
+        <is>
+          <t>vriezen</t>
+        </is>
+      </c>
+      <c r="C144" s="2" t="inlineStr">
+        <is>
+          <t>vroor, vroren</t>
+        </is>
+      </c>
+      <c r="E144" s="2" t="inlineStr">
+        <is>
+          <t>gevroren</t>
+        </is>
+      </c>
+      <c r="F144" s="2" t="inlineStr">
+        <is>
+          <t>freeze</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="145" s="3">
-      <c r="B145" s="2" t="n"/>
-      <c r="E145" s="2" t="n"/>
-      <c r="F145" s="2" t="n"/>
+      <c r="B145" s="2" t="inlineStr">
+        <is>
+          <t>waaien</t>
+        </is>
+      </c>
+      <c r="C145" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">waaide, waaiden, woei, woeien </t>
+        </is>
+      </c>
+      <c r="E145" s="2" t="inlineStr">
+        <is>
+          <t>gewaaid</t>
+        </is>
+      </c>
+      <c r="F145" s="2" t="inlineStr">
+        <is>
+          <t>blow</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="146" s="3">
-      <c r="B146" s="2" t="n"/>
-      <c r="E146" s="2" t="n"/>
-      <c r="F146" s="2" t="n"/>
+      <c r="B146" s="2" t="inlineStr">
+        <is>
+          <t>wassen</t>
+        </is>
+      </c>
+      <c r="C146" s="2" t="inlineStr">
+        <is>
+          <t>waste, wasten</t>
+        </is>
+      </c>
+      <c r="E146" s="2" t="inlineStr">
+        <is>
+          <t>gewassen</t>
+        </is>
+      </c>
+      <c r="F146" s="2" t="inlineStr">
+        <is>
+          <t>wash</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="147" s="3">
-      <c r="B147" s="2" t="n"/>
-      <c r="E147" s="2" t="n"/>
-      <c r="F147" s="2" t="n"/>
+      <c r="B147" s="2" t="inlineStr">
+        <is>
+          <t>wegen</t>
+        </is>
+      </c>
+      <c r="C147" s="2" t="inlineStr">
+        <is>
+          <t>woog, wogen</t>
+        </is>
+      </c>
+      <c r="E147" s="2" t="inlineStr">
+        <is>
+          <t>gewogen</t>
+        </is>
+      </c>
+      <c r="F147" s="2" t="inlineStr">
+        <is>
+          <t>weigh</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="148" s="3">
-      <c r="B148" s="2" t="n"/>
-      <c r="E148" s="2" t="n"/>
-      <c r="F148" s="2" t="n"/>
+      <c r="B148" s="2" t="inlineStr">
+        <is>
+          <t>werpen</t>
+        </is>
+      </c>
+      <c r="C148" s="2" t="inlineStr">
+        <is>
+          <t>wierp, wierpen</t>
+        </is>
+      </c>
+      <c r="E148" s="2" t="inlineStr">
+        <is>
+          <t>geworpen</t>
+        </is>
+      </c>
+      <c r="F148" s="2" t="inlineStr">
+        <is>
+          <t>throw</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="149" s="3">
-      <c r="B149" s="2" t="n"/>
-      <c r="E149" s="2" t="n"/>
-      <c r="F149" s="2" t="n"/>
+      <c r="B149" s="2" t="inlineStr">
+        <is>
+          <t>weten</t>
+        </is>
+      </c>
+      <c r="C149" s="2" t="inlineStr">
+        <is>
+          <t>wist, wisten</t>
+        </is>
+      </c>
+      <c r="E149" s="2" t="inlineStr">
+        <is>
+          <t>geweten</t>
+        </is>
+      </c>
+      <c r="F149" s="2" t="inlineStr">
+        <is>
+          <t>know</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="150" s="3">
-      <c r="B150" s="2" t="n"/>
-      <c r="E150" s="2" t="n"/>
-      <c r="F150" s="2" t="n"/>
+      <c r="B150" s="2" t="inlineStr">
+        <is>
+          <t>wijzen</t>
+        </is>
+      </c>
+      <c r="C150" s="2" t="inlineStr">
+        <is>
+          <t>wees, wezen</t>
+        </is>
+      </c>
+      <c r="E150" s="2" t="inlineStr">
+        <is>
+          <t>gewezen</t>
+        </is>
+      </c>
+      <c r="F150" s="2" t="inlineStr">
+        <is>
+          <t>show, point</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="151" s="3">
-      <c r="B151" s="2" t="n"/>
-      <c r="E151" s="2" t="n"/>
-      <c r="F151" s="2" t="n"/>
+      <c r="B151" s="2" t="inlineStr">
+        <is>
+          <t>willen</t>
+        </is>
+      </c>
+      <c r="C151" s="2" t="inlineStr">
+        <is>
+          <t>wilde / wou, wilden</t>
+        </is>
+      </c>
+      <c r="E151" s="2" t="inlineStr">
+        <is>
+          <t>gewild</t>
+        </is>
+      </c>
+      <c r="F151" s="2" t="inlineStr">
+        <is>
+          <t>want</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="152" s="3">
-      <c r="B152" s="2" t="n"/>
-      <c r="E152" s="2" t="n"/>
-      <c r="F152" s="2" t="n"/>
+      <c r="B152" s="2" t="inlineStr">
+        <is>
+          <t>winnen</t>
+        </is>
+      </c>
+      <c r="C152" s="2" t="inlineStr">
+        <is>
+          <t>won, wonnen</t>
+        </is>
+      </c>
+      <c r="E152" s="2" t="inlineStr">
+        <is>
+          <t>gewonnen</t>
+        </is>
+      </c>
+      <c r="F152" s="2" t="inlineStr">
+        <is>
+          <t>win</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="153" s="3">
-      <c r="B153" s="2" t="n"/>
-      <c r="D153" s="2" t="n"/>
-      <c r="E153" s="2" t="n"/>
-      <c r="F153" s="2" t="n"/>
+      <c r="B153" s="2" t="inlineStr">
+        <is>
+          <t>worden</t>
+        </is>
+      </c>
+      <c r="C153" s="2" t="inlineStr">
+        <is>
+          <t>werd, werden</t>
+        </is>
+      </c>
+      <c r="D153" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E153" s="2" t="inlineStr">
+        <is>
+          <t>geworden</t>
+        </is>
+      </c>
+      <c r="F153" s="2" t="inlineStr">
+        <is>
+          <t>become</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="154" s="3">
-      <c r="B154" s="2" t="n"/>
-      <c r="E154" s="2" t="n"/>
-      <c r="F154" s="2" t="n"/>
+      <c r="B154" s="2" t="inlineStr">
+        <is>
+          <t>wrijven</t>
+        </is>
+      </c>
+      <c r="C154" s="2" t="inlineStr">
+        <is>
+          <t>wreef, wreven</t>
+        </is>
+      </c>
+      <c r="E154" s="2" t="inlineStr">
+        <is>
+          <t>gewreven</t>
+        </is>
+      </c>
+      <c r="F154" s="2" t="inlineStr">
+        <is>
+          <t>rub</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="155" s="3">
-      <c r="B155" s="2" t="n"/>
-      <c r="E155" s="2" t="n"/>
-      <c r="F155" s="2" t="n"/>
+      <c r="B155" s="2" t="inlineStr">
+        <is>
+          <t>zeggen</t>
+        </is>
+      </c>
+      <c r="C155" s="2" t="inlineStr">
+        <is>
+          <t>zei, zeiden</t>
+        </is>
+      </c>
+      <c r="E155" s="2" t="inlineStr">
+        <is>
+          <t>gezegd</t>
+        </is>
+      </c>
+      <c r="F155" s="2" t="inlineStr">
+        <is>
+          <t>say</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="156" s="3">
-      <c r="B156" s="2" t="n"/>
-      <c r="E156" s="2" t="n"/>
-      <c r="F156" s="2" t="n"/>
+      <c r="B156" s="2" t="inlineStr">
+        <is>
+          <t>zenden</t>
+        </is>
+      </c>
+      <c r="C156" s="2" t="inlineStr">
+        <is>
+          <t>zond, zonden</t>
+        </is>
+      </c>
+      <c r="E156" s="2" t="inlineStr">
+        <is>
+          <t>gezonden</t>
+        </is>
+      </c>
+      <c r="F156" s="2" t="inlineStr">
+        <is>
+          <t>send</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="157" s="3">
-      <c r="B157" s="2" t="n"/>
-      <c r="E157" s="2" t="n"/>
-      <c r="F157" s="2" t="n"/>
+      <c r="B157" s="2" t="inlineStr">
+        <is>
+          <t>zien</t>
+        </is>
+      </c>
+      <c r="C157" s="2" t="inlineStr">
+        <is>
+          <t>zag, zagen</t>
+        </is>
+      </c>
+      <c r="E157" s="2" t="inlineStr">
+        <is>
+          <t>gezien</t>
+        </is>
+      </c>
+      <c r="F157" s="2" t="inlineStr">
+        <is>
+          <t>see</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="158" s="3">
-      <c r="B158" s="2" t="n"/>
-      <c r="D158" s="2" t="n"/>
-      <c r="E158" s="2" t="n"/>
-      <c r="F158" s="2" t="n"/>
+      <c r="B158" s="2" t="inlineStr">
+        <is>
+          <t>zijn</t>
+        </is>
+      </c>
+      <c r="C158" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">was, waren </t>
+        </is>
+      </c>
+      <c r="D158" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E158" s="2" t="inlineStr">
+        <is>
+          <t>geweest</t>
+        </is>
+      </c>
+      <c r="F158" s="2" t="inlineStr">
+        <is>
+          <t>be</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="159" s="3">
-      <c r="B159" s="2" t="n"/>
-      <c r="E159" s="2" t="n"/>
-      <c r="F159" s="2" t="n"/>
+      <c r="B159" s="2" t="inlineStr">
+        <is>
+          <t>zingen</t>
+        </is>
+      </c>
+      <c r="C159" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">zong, zongen </t>
+        </is>
+      </c>
+      <c r="E159" s="2" t="inlineStr">
+        <is>
+          <t>gezongen</t>
+        </is>
+      </c>
+      <c r="F159" s="2" t="inlineStr">
+        <is>
+          <t>sing</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="160" s="3">
-      <c r="B160" s="2" t="n"/>
-      <c r="D160" s="2" t="n"/>
-      <c r="E160" s="2" t="n"/>
-      <c r="F160" s="2" t="n"/>
+      <c r="B160" s="2" t="inlineStr">
+        <is>
+          <t>zinken</t>
+        </is>
+      </c>
+      <c r="C160" s="2" t="inlineStr">
+        <is>
+          <t>zonk, zonken</t>
+        </is>
+      </c>
+      <c r="D160" s="2" t="inlineStr">
+        <is>
+          <t>is</t>
+        </is>
+      </c>
+      <c r="E160" s="2" t="inlineStr">
+        <is>
+          <t>gezonken</t>
+        </is>
+      </c>
+      <c r="F160" s="2" t="inlineStr">
+        <is>
+          <t>sink</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="161" s="3">
-      <c r="B161" s="2" t="n"/>
-      <c r="E161" s="2" t="n"/>
-      <c r="F161" s="2" t="n"/>
+      <c r="B161" s="2" t="inlineStr">
+        <is>
+          <t>zitten</t>
+        </is>
+      </c>
+      <c r="C161" s="2" t="inlineStr">
+        <is>
+          <t>zat, zaten</t>
+        </is>
+      </c>
+      <c r="E161" s="2" t="inlineStr">
+        <is>
+          <t>gezeten</t>
+        </is>
+      </c>
+      <c r="F161" s="2" t="inlineStr">
+        <is>
+          <t>sit</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="162" s="3">
-      <c r="B162" s="2" t="n"/>
-      <c r="E162" s="2" t="n"/>
-      <c r="F162" s="2" t="n"/>
+      <c r="B162" s="2" t="inlineStr">
+        <is>
+          <t>zoeken</t>
+        </is>
+      </c>
+      <c r="C162" s="2" t="inlineStr">
+        <is>
+          <t>zocht, zochten</t>
+        </is>
+      </c>
+      <c r="E162" s="2" t="inlineStr">
+        <is>
+          <t>gezocht</t>
+        </is>
+      </c>
+      <c r="F162" s="2" t="inlineStr">
+        <is>
+          <t>search, look</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="163" s="3">
-      <c r="B163" s="2" t="n"/>
-      <c r="E163" s="2" t="n"/>
-      <c r="F163" s="2" t="n"/>
+      <c r="B163" s="2" t="inlineStr">
+        <is>
+          <t>zullen</t>
+        </is>
+      </c>
+      <c r="C163" s="2" t="inlineStr">
+        <is>
+          <t>zou, zouden</t>
+        </is>
+      </c>
+      <c r="E163" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F163" s="2" t="inlineStr">
+        <is>
+          <t>will, would</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="164" s="3">
-      <c r="B164" s="2" t="n"/>
-      <c r="D164" s="2" t="n"/>
-      <c r="E164" s="2" t="n"/>
-      <c r="F164" s="2" t="n"/>
+      <c r="B164" s="2" t="inlineStr">
+        <is>
+          <t>zwemmen</t>
+        </is>
+      </c>
+      <c r="C164" s="2" t="inlineStr">
+        <is>
+          <t>zwom, zwommen</t>
+        </is>
+      </c>
+      <c r="D164" s="2" t="inlineStr">
+        <is>
+          <t>(is)</t>
+        </is>
+      </c>
+      <c r="E164" s="2" t="inlineStr">
+        <is>
+          <t>gezwommen</t>
+        </is>
+      </c>
+      <c r="F164" s="2" t="inlineStr">
+        <is>
+          <t>swim</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="165" s="3">
-      <c r="B165" s="2" t="n"/>
-      <c r="D165" s="2" t="n"/>
-      <c r="E165" s="2" t="n"/>
-      <c r="F165" s="2" t="n"/>
+      <c r="B165" s="2" t="inlineStr">
+        <is>
+          <t>zweren</t>
+        </is>
+      </c>
+      <c r="C165" s="4" t="inlineStr">
+        <is>
+          <t>zwoer, zwoeren</t>
+        </is>
+      </c>
+      <c r="D165" s="4" t="n"/>
+      <c r="E165" s="2" t="inlineStr">
+        <is>
+          <t>gezworen</t>
+        </is>
+      </c>
+      <c r="F165" s="2" t="inlineStr">
+        <is>
+          <t>swear</t>
+        </is>
+      </c>
     </row>
     <row customHeight="1" ht="12.8" r="166" s="3">
-      <c r="B166" s="2" t="n"/>
-      <c r="E166" s="2" t="n"/>
-      <c r="F166" s="2" t="n"/>
+      <c r="B166" s="2" t="inlineStr">
+        <is>
+          <t>zwijgen</t>
+        </is>
+      </c>
+      <c r="C166" s="2" t="inlineStr">
+        <is>
+          <t>zweeg, zwegen</t>
+        </is>
+      </c>
+      <c r="E166" s="2" t="inlineStr">
+        <is>
+          <t>gezwegen</t>
+        </is>
+      </c>
+      <c r="F166" s="2" t="inlineStr">
+        <is>
+          <t>be silent</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
@@ -3703,12 +4504,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A27" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="B123:C123 A2"/>
+      <selection activeCell="A2" activeCellId="1" pane="topLeft" sqref="B139:F166 A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="2" width="15.8"/>
+    <col customWidth="1" max="2" min="2" style="2" width="15.79"/>
     <col customWidth="1" max="5" min="5" style="2" width="14.76"/>
   </cols>
   <sheetData>
@@ -4448,10 +5249,10 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A12" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A12" activeCellId="1" pane="topLeft" sqref="B123:C123 A12"/>
+      <selection activeCell="A12" activeCellId="1" pane="topLeft" sqref="B139:F166 A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="15.48"/>
   </cols>
@@ -5050,10 +5851,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="17.06"/>
   </cols>
@@ -5312,12 +6113,12 @@
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A36" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col customWidth="1" max="2" min="2" style="2" width="25.21"/>
+    <col customWidth="1" max="2" min="2" style="2" width="25.22"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="12.8" r="1" s="3">
@@ -6291,10 +7092,10 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A30" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="20.74"/>
     <col customWidth="1" max="5" min="5" style="2" width="17.54"/>
@@ -7308,10 +8109,10 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="0" topLeftCell="A19" view="normal" workbookViewId="0" zoomScale="179" zoomScaleNormal="179" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B123:C123 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B139:F166 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.58984375" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
     <col customWidth="1" max="2" min="2" style="2" width="27.65"/>
   </cols>
@@ -7914,12 +8715,12 @@
           <t>zweren</t>
         </is>
       </c>
-      <c r="B27" s="2" t="inlineStr">
+      <c r="B27" s="4" t="inlineStr">
         <is>
           <t>zwoer, zwoeren</t>
         </is>
       </c>
-      <c r="C27" s="2" t="n"/>
+      <c r="C27" s="4" t="n"/>
       <c r="D27" s="2" t="inlineStr">
         <is>
           <t>gezworen</t>

</xml_diff>

<commit_message>
Add note edit area
Spell checker of note will be added later.
</commit_message>
<xml_diff>
--- a/Werkwoorden_Lijst.xlsx
+++ b/Werkwoorden_Lijst.xlsx
@@ -13,19 +13,19 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Frequent1 " sheetId="2" r:id="rId2"/>
+    <sheet name="Frequent2" sheetId="3" r:id="rId3"/>
+    <sheet name="Infrequent1" sheetId="4" r:id="rId4"/>
+    <sheet name="Infrequent2" sheetId="5" r:id="rId5"/>
+    <sheet name="Infrequent3" sheetId="6" r:id="rId6"/>
+    <sheet name="Infrequent4" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="515">
   <si>
     <t>Stam</t>
   </si>
@@ -1917,7 +1917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -4604,8 +4604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="A2" activeCellId="1" sqref="B139:F166 A2"/>
+    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5078,10 +5078,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCell="A12" activeCellId="1" sqref="B139:F166 A12"/>
+    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5089,367 +5089,375 @@
     <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>287</v>
+        <v>490</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>288</v>
+        <v>491</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>289</v>
+        <v>492</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>290</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>288</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>334</v>
+        <v>294</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>335</v>
+        <v>295</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>336</v>
+        <v>296</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>337</v>
+        <v>297</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>393</v>
+        <v>370</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>394</v>
+        <v>371</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>395</v>
+        <v>372</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>496</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>399</v>
+        <v>496</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>497</v>
+        <v>398</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>128</v>
+        <v>400</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>401</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>130</v>
+        <v>497</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>131</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>152</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>182</v>
-      </c>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -5463,10 +5471,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCellId="1" sqref="B139:F166 A1"/>
+      <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5474,149 +5482,166 @@
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>490</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>491</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>492</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>186</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>498</v>
+        <v>188</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>499</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>500</v>
+        <v>189</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>501</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>502</v>
+        <v>498</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>499</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>191</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>192</v>
+        <v>502</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>193</v>
+        <v>503</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>194</v>
+        <v>504</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>203</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>505</v>
+        <v>204</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>506</v>
+        <v>205</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>507</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>210</v>
       </c>
     </row>
@@ -5632,10 +5657,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCellId="1" sqref="B139:F166 A1"/>
+    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5643,604 +5668,621 @@
     <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>490</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>212</v>
+        <v>491</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>213</v>
+        <v>492</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>214</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>211</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>212</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>20</v>
+        <v>213</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>508</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>215</v>
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>216</v>
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>217</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>218</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>219</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>220</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>221</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>223</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>225</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>226</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>26</v>
+        <v>223</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>225</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>29</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>227</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>117</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>229</v>
+        <v>45</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>230</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>227</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>228</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>49</v>
+        <v>229</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>50</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>231</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>232</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>233</v>
+        <v>49</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>234</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>231</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>232</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>233</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>235</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>236</v>
+        <v>52</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>237</v>
+        <v>53</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>238</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>235</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>236</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>237</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>58</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>239</v>
+        <v>55</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>240</v>
+        <v>56</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>241</v>
+        <v>57</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>242</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>240</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>60</v>
+        <v>256</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>61</v>
+        <v>257</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>62</v>
+        <v>258</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>259</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>260</v>
+        <v>64</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>261</v>
+        <v>65</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>262</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>67</v>
+        <v>259</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>68</v>
+        <v>260</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>69</v>
+        <v>261</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>70</v>
+        <v>262</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>263</v>
+        <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>264</v>
+        <v>68</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>265</v>
+        <v>69</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>266</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>71</v>
+        <v>263</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>264</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>73</v>
+        <v>265</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>74</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>267</v>
+        <v>75</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>269</v>
+        <v>77</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>270</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>79</v>
+        <v>271</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
+        <v>272</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>81</v>
+        <v>273</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>82</v>
+        <v>274</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>275</v>
+        <v>87</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>277</v>
+        <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>278</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>91</v>
+        <v>279</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>92</v>
+        <v>280</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>93</v>
+        <v>281</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>94</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D42" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>510</v>
       </c>
     </row>
@@ -6256,10 +6298,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCellId="1" sqref="B139:F166 A1"/>
+    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6268,627 +6310,644 @@
     <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>111</v>
+        <v>490</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>511</v>
+        <v>491</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>113</v>
+        <v>492</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>510</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>283</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>284</v>
+        <v>511</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>285</v>
+        <v>113</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>286</v>
+        <v>510</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>115</v>
+        <v>283</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>117</v>
+        <v>284</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>118</v>
+        <v>285</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>119</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>512</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>287</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>288</v>
+        <v>125</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>289</v>
+        <v>126</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>290</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>181</v>
+        <v>289</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>117</v>
+        <v>292</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>296</v>
+        <v>181</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>335</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>363</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>371</v>
+        <v>367</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>7</v>
+        <v>379</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>270</v>
+        <v>385</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>392</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>349</v>
+        <v>392</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>399</v>
+        <v>349</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>405</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>128</v>
+        <v>408</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>129</v>
+        <v>409</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>117</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>130</v>
+        <v>410</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>131</v>
+        <v>411</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>412</v>
+        <v>128</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>413</v>
+        <v>129</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>414</v>
+        <v>130</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>415</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>7</v>
+        <v>413</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>416</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>133</v>
+        <v>417</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>132</v>
+        <v>418</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>134</v>
+        <v>419</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E43" s="1" t="s">
         <v>138</v>
       </c>
     </row>
@@ -6904,10 +6963,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
-      <selection activeCellId="1" sqref="B139:F166 A1"/>
+    <sheetView zoomScale="179" zoomScaleNormal="179" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6915,408 +6974,425 @@
     <col min="2" max="2" width="27.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>420</v>
+        <v>490</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>421</v>
+        <v>491</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>422</v>
+        <v>492</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>423</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>420</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>140</v>
+        <v>421</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>141</v>
+        <v>422</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>142</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>424</v>
+        <v>139</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>425</v>
+        <v>140</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>426</v>
+        <v>141</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>427</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>143</v>
+        <v>428</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>429</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>145</v>
+        <v>430</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>146</v>
+        <v>431</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>432</v>
+        <v>143</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>433</v>
+        <v>144</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>434</v>
+        <v>145</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>435</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>147</v>
+        <v>448</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>148</v>
+        <v>449</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>149</v>
+        <v>450</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>150</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>452</v>
+        <v>147</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>453</v>
+        <v>148</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>454</v>
+        <v>149</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>455</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>151</v>
+        <v>452</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>488</v>
+        <v>453</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>153</v>
+        <v>454</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>154</v>
+        <v>455</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>456</v>
+        <v>151</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>457</v>
+        <v>488</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>458</v>
+        <v>153</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>459</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>155</v>
+        <v>456</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>7</v>
+        <v>457</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>157</v>
+        <v>458</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>158</v>
+        <v>459</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>460</v>
+        <v>155</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>461</v>
+        <v>156</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>462</v>
+        <v>157</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>463</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>159</v>
+        <v>460</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>160</v>
+        <v>461</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>161</v>
+        <v>462</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>162</v>
+        <v>463</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>464</v>
+        <v>159</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>465</v>
+        <v>160</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>466</v>
+        <v>161</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>467</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>163</v>
+        <v>464</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>164</v>
+        <v>465</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>165</v>
+        <v>466</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>166</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>468</v>
+        <v>167</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>469</v>
+        <v>489</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>470</v>
+        <v>169</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>471</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
+        <v>469</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>171</v>
+        <v>472</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>172</v>
+        <v>473</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>173</v>
+        <v>474</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>174</v>
+        <v>475</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>476</v>
+        <v>179</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>478</v>
+        <v>181</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>479</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>480</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>476</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>117</v>
+      </c>
       <c r="D27" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
         <v>484</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D29" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>487</v>
       </c>
     </row>

</xml_diff>